<commit_message>
update and make consistent the code
</commit_message>
<xml_diff>
--- a/02_PersistenceOfVision/Pattern_Calcs.xlsx
+++ b/02_PersistenceOfVision/Pattern_Calcs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8A1FA3-482D-42A3-B89D-D5ADAD6A95DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0C902A-9224-421C-8E07-DC426E2502FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10170" yWindow="5790" windowWidth="25515" windowHeight="14295" activeTab="1" xr2:uid="{4F6297C5-B3B5-48D5-ADDF-AF5E88E5519F}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="25515" windowHeight="14295" activeTab="1" xr2:uid="{4F6297C5-B3B5-48D5-ADDF-AF5E88E5519F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ovals" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="30">
   <si>
     <t>X</t>
   </si>
@@ -86,12 +86,6 @@
     <t>0x7E</t>
   </si>
   <si>
-    <t>0xE0</t>
-  </si>
-  <si>
-    <t>0x1E</t>
-  </si>
-  <si>
     <t>0x98</t>
   </si>
   <si>
@@ -107,10 +101,16 @@
     <t>0xF9</t>
   </si>
   <si>
-    <t xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { </t>
+    <t xml:space="preserve">  static unsigned int oval_pattern[OVAL_CALLS_THEN_REPEAT] = { </t>
   </si>
   <si>
-    <t xml:space="preserve">  static unsigned int oval_pattern[OVAL_CALLS_THEN_REPEAT] = { </t>
+    <t>0xFE</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { </t>
   </si>
 </sst>
 </file>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="BC7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:87" x14ac:dyDescent="0.25">
@@ -1451,19 +1451,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AAAADA-9358-4C28-B2E0-ECDDA6F974A8}">
-  <dimension ref="A1:DM65"/>
+  <dimension ref="A1:DI62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BI7" sqref="BI7"/>
+      <selection activeCell="BF12" sqref="BF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="58" width="2.140625" customWidth="1"/>
+    <col min="2" max="55" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1503,267 +1503,252 @@
       <c r="AI1" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AJ1" t="s">
         <v>0</v>
       </c>
       <c r="AM1" t="s">
         <v>0</v>
       </c>
-      <c r="AP1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ1" t="s">
+      <c r="AN1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO1" t="s">
         <v>0</v>
       </c>
       <c r="AR1" t="s">
         <v>0</v>
       </c>
-      <c r="AU1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH1" t="str">
+      <c r="AW1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG1" t="str">
         <f>LEN(A1)&amp;LEN(A2)&amp;LEN(A3)&amp;LEN(A4)&amp;LEN(A5)&amp;LEN(A6)&amp;LEN(A7)&amp;LEN(A8)</f>
         <v>11111111</v>
       </c>
+      <c r="BH1" t="str">
+        <f>LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
+        <v>00011000</v>
+      </c>
       <c r="BI1" t="str">
-        <f t="shared" ref="BI1:DH1" si="0">LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
+        <f>LEN(C1)&amp;LEN(C2)&amp;LEN(C3)&amp;LEN(C4)&amp;LEN(C5)&amp;LEN(C6)&amp;LEN(C7)&amp;LEN(C8)</f>
         <v>00011000</v>
       </c>
       <c r="BJ1" t="str">
-        <f t="shared" si="0"/>
+        <f>LEN(D1)&amp;LEN(D2)&amp;LEN(D3)&amp;LEN(D4)&amp;LEN(D5)&amp;LEN(D6)&amp;LEN(D7)&amp;LEN(D8)</f>
         <v>00011000</v>
       </c>
       <c r="BK1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011000</v>
+        <f>LEN(E1)&amp;LEN(E2)&amp;LEN(E3)&amp;LEN(E4)&amp;LEN(E5)&amp;LEN(E6)&amp;LEN(E7)&amp;LEN(E8)</f>
+        <v>11111111</v>
       </c>
       <c r="BL1" t="str">
-        <f t="shared" si="0"/>
+        <f>LEN(F1)&amp;LEN(F2)&amp;LEN(F3)&amp;LEN(F4)&amp;LEN(F5)&amp;LEN(F6)&amp;LEN(F7)&amp;LEN(F8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="BM1" t="str">
+        <f>LEN(G1)&amp;LEN(G2)&amp;LEN(G3)&amp;LEN(G4)&amp;LEN(G5)&amp;LEN(G6)&amp;LEN(G7)&amp;LEN(G8)</f>
         <v>11111111</v>
       </c>
-      <c r="BM1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BN1" t="str">
+        <f>LEN(H1)&amp;LEN(H2)&amp;LEN(H3)&amp;LEN(H4)&amp;LEN(H5)&amp;LEN(H6)&amp;LEN(H7)&amp;LEN(H8)</f>
+        <v>10001001</v>
+      </c>
+      <c r="BO1" t="str">
+        <f>LEN(I1)&amp;LEN(I2)&amp;LEN(I3)&amp;LEN(I4)&amp;LEN(I5)&amp;LEN(I6)&amp;LEN(I7)&amp;LEN(I8)</f>
+        <v>10001001</v>
+      </c>
+      <c r="BP1" t="str">
+        <f>LEN(J1)&amp;LEN(J2)&amp;LEN(J3)&amp;LEN(J4)&amp;LEN(J5)&amp;LEN(J6)&amp;LEN(J7)&amp;LEN(J8)</f>
+        <v>10001001</v>
+      </c>
+      <c r="BQ1" t="str">
+        <f>LEN(K1)&amp;LEN(K2)&amp;LEN(K3)&amp;LEN(K4)&amp;LEN(K5)&amp;LEN(K6)&amp;LEN(K7)&amp;LEN(K8)</f>
         <v>00000000</v>
       </c>
-      <c r="BN1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BR1" t="str">
+        <f>LEN(L1)&amp;LEN(L2)&amp;LEN(L3)&amp;LEN(L4)&amp;LEN(L5)&amp;LEN(L6)&amp;LEN(L7)&amp;LEN(L8)</f>
         <v>11111111</v>
       </c>
-      <c r="BO1" t="str">
-        <f t="shared" si="0"/>
-        <v>10001001</v>
-      </c>
-      <c r="BP1" t="str">
-        <f t="shared" si="0"/>
-        <v>10001001</v>
-      </c>
-      <c r="BQ1" t="str">
-        <f t="shared" si="0"/>
-        <v>10001001</v>
-      </c>
-      <c r="BR1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BS1" t="str">
+        <f>LEN(M1)&amp;LEN(M2)&amp;LEN(M3)&amp;LEN(M4)&amp;LEN(M5)&amp;LEN(M6)&amp;LEN(M7)&amp;LEN(M8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="BT1" t="str">
+        <f>LEN(N1)&amp;LEN(N2)&amp;LEN(N3)&amp;LEN(N4)&amp;LEN(N5)&amp;LEN(N6)&amp;LEN(N7)&amp;LEN(N8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="BU1" t="str">
+        <f>LEN(O1)&amp;LEN(O2)&amp;LEN(O3)&amp;LEN(O4)&amp;LEN(O5)&amp;LEN(O6)&amp;LEN(O7)&amp;LEN(O8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="BV1" t="str">
+        <f>LEN(P1)&amp;LEN(P2)&amp;LEN(P3)&amp;LEN(P4)&amp;LEN(P5)&amp;LEN(P6)&amp;LEN(P7)&amp;LEN(P8)</f>
         <v>00000000</v>
       </c>
-      <c r="BS1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BW1" t="str">
+        <f>LEN(Q1)&amp;LEN(Q2)&amp;LEN(Q3)&amp;LEN(Q4)&amp;LEN(Q5)&amp;LEN(Q6)&amp;LEN(Q7)&amp;LEN(Q8)</f>
         <v>11111111</v>
       </c>
-      <c r="BT1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BX1" t="str">
+        <f>LEN(R1)&amp;LEN(R2)&amp;LEN(R3)&amp;LEN(R4)&amp;LEN(R5)&amp;LEN(R6)&amp;LEN(R7)&amp;LEN(R8)</f>
         <v>00000001</v>
       </c>
-      <c r="BU1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BY1" t="str">
+        <f>LEN(S1)&amp;LEN(S2)&amp;LEN(S3)&amp;LEN(S4)&amp;LEN(S5)&amp;LEN(S6)&amp;LEN(S7)&amp;LEN(S8)</f>
         <v>00000001</v>
       </c>
-      <c r="BV1" t="str">
-        <f t="shared" si="0"/>
+      <c r="BZ1" t="str">
+        <f>LEN(T1)&amp;LEN(T2)&amp;LEN(T3)&amp;LEN(T4)&amp;LEN(T5)&amp;LEN(T6)&amp;LEN(T7)&amp;LEN(T8)</f>
         <v>00000001</v>
       </c>
-      <c r="BW1" t="str">
-        <f t="shared" si="0"/>
+      <c r="CA1" t="str">
+        <f>LEN(U1)&amp;LEN(U2)&amp;LEN(U3)&amp;LEN(U4)&amp;LEN(U5)&amp;LEN(U6)&amp;LEN(U7)&amp;LEN(U8)</f>
         <v>00000000</v>
       </c>
-      <c r="BX1" t="str">
-        <f t="shared" si="0"/>
+      <c r="CB1" t="str">
+        <f>LEN(V1)&amp;LEN(V2)&amp;LEN(V3)&amp;LEN(V4)&amp;LEN(V5)&amp;LEN(V6)&amp;LEN(V7)&amp;LEN(V8)</f>
+        <v>01111110</v>
+      </c>
+      <c r="CC1" t="str">
+        <f>LEN(W1)&amp;LEN(W2)&amp;LEN(W3)&amp;LEN(W4)&amp;LEN(W5)&amp;LEN(W6)&amp;LEN(W7)&amp;LEN(W8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="CD1" t="str">
+        <f>LEN(X1)&amp;LEN(X2)&amp;LEN(X3)&amp;LEN(X4)&amp;LEN(X5)&amp;LEN(X6)&amp;LEN(X7)&amp;LEN(X8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="CE1" t="str">
+        <f>LEN(Y1)&amp;LEN(Y2)&amp;LEN(Y3)&amp;LEN(Y4)&amp;LEN(Y5)&amp;LEN(Y6)&amp;LEN(Y7)&amp;LEN(Y8)</f>
+        <v>01111110</v>
+      </c>
+      <c r="CF1" t="str">
+        <f>LEN(Z1)&amp;LEN(Z2)&amp;LEN(Z3)&amp;LEN(Z4)&amp;LEN(Z5)&amp;LEN(Z6)&amp;LEN(Z7)&amp;LEN(Z8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="CG1" t="str">
+        <f>LEN(AA1)&amp;LEN(AA2)&amp;LEN(AA3)&amp;LEN(AA4)&amp;LEN(AA5)&amp;LEN(AA6)&amp;LEN(AA7)&amp;LEN(AA8)</f>
+        <v>11111110</v>
+      </c>
+      <c r="CH1" t="str">
+        <f>LEN(AB1)&amp;LEN(AB2)&amp;LEN(AB3)&amp;LEN(AB4)&amp;LEN(AB5)&amp;LEN(AB6)&amp;LEN(AB7)&amp;LEN(AB8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="CI1" t="str">
+        <f>LEN(AC1)&amp;LEN(AC2)&amp;LEN(AC3)&amp;LEN(AC4)&amp;LEN(AC5)&amp;LEN(AC6)&amp;LEN(AC7)&amp;LEN(AC8)</f>
+        <v>00001110</v>
+      </c>
+      <c r="CJ1" t="str">
+        <f>LEN(AD1)&amp;LEN(AD2)&amp;LEN(AD3)&amp;LEN(AD4)&amp;LEN(AD5)&amp;LEN(AD6)&amp;LEN(AD7)&amp;LEN(AD8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="CK1" t="str">
+        <f>LEN(AE1)&amp;LEN(AE2)&amp;LEN(AE3)&amp;LEN(AE4)&amp;LEN(AE5)&amp;LEN(AE6)&amp;LEN(AE7)&amp;LEN(AE8)</f>
+        <v>11111110</v>
+      </c>
+      <c r="CL1" t="str">
+        <f>LEN(AF1)&amp;LEN(AF2)&amp;LEN(AF3)&amp;LEN(AF4)&amp;LEN(AF5)&amp;LEN(AF6)&amp;LEN(AF7)&amp;LEN(AF8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="CM1" t="str">
+        <f>LEN(AG1)&amp;LEN(AG2)&amp;LEN(AG3)&amp;LEN(AG4)&amp;LEN(AG5)&amp;LEN(AG6)&amp;LEN(AG7)&amp;LEN(AG8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="CN1" t="str">
+        <f>LEN(AH1)&amp;LEN(AH2)&amp;LEN(AH3)&amp;LEN(AH4)&amp;LEN(AH5)&amp;LEN(AH6)&amp;LEN(AH7)&amp;LEN(AH8)</f>
+        <v>01111110</v>
+      </c>
+      <c r="CO1" t="str">
+        <f>LEN(AI1)&amp;LEN(AI2)&amp;LEN(AI3)&amp;LEN(AI4)&amp;LEN(AI5)&amp;LEN(AI6)&amp;LEN(AI7)&amp;LEN(AI8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="CP1" t="str">
+        <f>LEN(AJ1)&amp;LEN(AJ2)&amp;LEN(AJ3)&amp;LEN(AJ4)&amp;LEN(AJ5)&amp;LEN(AJ6)&amp;LEN(AJ7)&amp;LEN(AJ8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="CQ1" t="str">
+        <f>LEN(AK1)&amp;LEN(AK2)&amp;LEN(AK3)&amp;LEN(AK4)&amp;LEN(AK5)&amp;LEN(AK6)&amp;LEN(AK7)&amp;LEN(AK8)</f>
+        <v>01111110</v>
+      </c>
+      <c r="CR1" t="str">
+        <f>LEN(AL1)&amp;LEN(AL2)&amp;LEN(AL3)&amp;LEN(AL4)&amp;LEN(AL5)&amp;LEN(AL6)&amp;LEN(AL7)&amp;LEN(AL8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="CS1" t="str">
+        <f>LEN(AM1)&amp;LEN(AM2)&amp;LEN(AM3)&amp;LEN(AM4)&amp;LEN(AM5)&amp;LEN(AM6)&amp;LEN(AM7)&amp;LEN(AM8)</f>
         <v>11111111</v>
       </c>
-      <c r="BY1" t="str">
-        <f t="shared" si="0"/>
+      <c r="CT1" t="str">
+        <f>LEN(AN1)&amp;LEN(AN2)&amp;LEN(AN3)&amp;LEN(AN4)&amp;LEN(AN5)&amp;LEN(AN6)&amp;LEN(AN7)&amp;LEN(AN8)</f>
+        <v>10011000</v>
+      </c>
+      <c r="CU1" t="str">
+        <f>LEN(AO1)&amp;LEN(AO2)&amp;LEN(AO3)&amp;LEN(AO4)&amp;LEN(AO5)&amp;LEN(AO6)&amp;LEN(AO7)&amp;LEN(AO8)</f>
+        <v>10010100</v>
+      </c>
+      <c r="CV1" t="str">
+        <f>LEN(AP1)&amp;LEN(AP2)&amp;LEN(AP3)&amp;LEN(AP4)&amp;LEN(AP5)&amp;LEN(AP6)&amp;LEN(AP7)&amp;LEN(AP8)</f>
+        <v>01100011</v>
+      </c>
+      <c r="CW1" t="str">
+        <f>LEN(AQ1)&amp;LEN(AQ2)&amp;LEN(AQ3)&amp;LEN(AQ4)&amp;LEN(AQ5)&amp;LEN(AQ6)&amp;LEN(AQ7)&amp;LEN(AQ8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="CX1" t="str">
+        <f>LEN(AR1)&amp;LEN(AR2)&amp;LEN(AR3)&amp;LEN(AR4)&amp;LEN(AR5)&amp;LEN(AR6)&amp;LEN(AR7)&amp;LEN(AR8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="CY1" t="str">
+        <f>LEN(AS1)&amp;LEN(AS2)&amp;LEN(AS3)&amp;LEN(AS4)&amp;LEN(AS5)&amp;LEN(AS6)&amp;LEN(AS7)&amp;LEN(AS8)</f>
         <v>00000001</v>
       </c>
-      <c r="BZ1" t="str">
-        <f t="shared" si="0"/>
+      <c r="CZ1" t="str">
+        <f>LEN(AT1)&amp;LEN(AT2)&amp;LEN(AT3)&amp;LEN(AT4)&amp;LEN(AT5)&amp;LEN(AT6)&amp;LEN(AT7)&amp;LEN(AT8)</f>
         <v>00000001</v>
       </c>
-      <c r="CA1" t="str">
-        <f t="shared" si="0"/>
+      <c r="DA1" t="str">
+        <f>LEN(AU1)&amp;LEN(AU2)&amp;LEN(AU3)&amp;LEN(AU4)&amp;LEN(AU5)&amp;LEN(AU6)&amp;LEN(AU7)&amp;LEN(AU8)</f>
         <v>00000001</v>
       </c>
-      <c r="CB1" t="str">
-        <f t="shared" si="0"/>
+      <c r="DB1" t="str">
+        <f>LEN(AV1)&amp;LEN(AV2)&amp;LEN(AV3)&amp;LEN(AV4)&amp;LEN(AV5)&amp;LEN(AV6)&amp;LEN(AV7)&amp;LEN(AV8)</f>
         <v>00000000</v>
       </c>
-      <c r="CC1" t="str">
-        <f t="shared" si="0"/>
-        <v>01111110</v>
-      </c>
-      <c r="CD1" t="str">
-        <f t="shared" si="0"/>
+      <c r="DC1" t="str">
+        <f>LEN(AW1)&amp;LEN(AW2)&amp;LEN(AW3)&amp;LEN(AW4)&amp;LEN(AW5)&amp;LEN(AW6)&amp;LEN(AW7)&amp;LEN(AW8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="DD1" t="str">
+        <f>LEN(AX1)&amp;LEN(AX2)&amp;LEN(AX3)&amp;LEN(AX4)&amp;LEN(AX5)&amp;LEN(AX6)&amp;LEN(AX7)&amp;LEN(AX8)</f>
         <v>10000001</v>
       </c>
-      <c r="CE1" t="str">
-        <f t="shared" si="0"/>
-        <v>10000001</v>
-      </c>
-      <c r="CF1" t="str">
-        <f t="shared" si="0"/>
-        <v>01111110</v>
-      </c>
-      <c r="CG1" t="str">
-        <f t="shared" si="0"/>
+      <c r="DE1" t="str">
+        <f>LEN(AY1)&amp;LEN(AY2)&amp;LEN(AY3)&amp;LEN(AY4)&amp;LEN(AY5)&amp;LEN(AY6)&amp;LEN(AY7)&amp;LEN(AY8)</f>
+        <v>01000010</v>
+      </c>
+      <c r="DF1" t="str">
+        <f>LEN(AZ1)&amp;LEN(AZ2)&amp;LEN(AZ3)&amp;LEN(AZ4)&amp;LEN(AZ5)&amp;LEN(AZ6)&amp;LEN(AZ7)&amp;LEN(AZ8)</f>
+        <v>00111100</v>
+      </c>
+      <c r="DG1" t="str">
+        <f>LEN(BA1)&amp;LEN(BA2)&amp;LEN(BA3)&amp;LEN(BA4)&amp;LEN(BA5)&amp;LEN(BA6)&amp;LEN(BA7)&amp;LEN(BA8)</f>
         <v>00000000</v>
       </c>
-      <c r="CH1" t="str">
-        <f t="shared" si="0"/>
-        <v>11100000</v>
-      </c>
-      <c r="CI1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011110</v>
-      </c>
-      <c r="CJ1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000001</v>
-      </c>
-      <c r="CK1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011110</v>
-      </c>
-      <c r="CL1" t="str">
-        <f t="shared" si="0"/>
-        <v>11100000</v>
-      </c>
-      <c r="CM1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011110</v>
-      </c>
-      <c r="CN1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000001</v>
-      </c>
-      <c r="CO1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011110</v>
-      </c>
-      <c r="CP1" t="str">
-        <f t="shared" si="0"/>
-        <v>11100000</v>
-      </c>
-      <c r="CQ1" t="str">
-        <f t="shared" si="0"/>
+      <c r="DH1" t="str">
+        <f>LEN(BB1)&amp;LEN(BB2)&amp;LEN(BB3)&amp;LEN(BB4)&amp;LEN(BB5)&amp;LEN(BB6)&amp;LEN(BB7)&amp;LEN(BB8)</f>
+        <v>11111001</v>
+      </c>
+      <c r="DI1" t="str">
+        <f>LEN(BC1)&amp;LEN(BC2)&amp;LEN(BC3)&amp;LEN(BC4)&amp;LEN(BC5)&amp;LEN(BC6)&amp;LEN(BC7)&amp;LEN(BC8)</f>
         <v>00000000</v>
       </c>
-      <c r="CR1" t="str">
-        <f t="shared" si="0"/>
-        <v>01111110</v>
-      </c>
-      <c r="CS1" t="str">
-        <f t="shared" si="0"/>
-        <v>10000001</v>
-      </c>
-      <c r="CT1" t="str">
-        <f t="shared" si="0"/>
-        <v>10000001</v>
-      </c>
-      <c r="CU1" t="str">
-        <f t="shared" si="0"/>
-        <v>01111110</v>
-      </c>
-      <c r="CV1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
-      </c>
-      <c r="CW1" t="str">
-        <f t="shared" si="0"/>
-        <v>11111111</v>
-      </c>
-      <c r="CX1" t="str">
-        <f t="shared" si="0"/>
-        <v>10011000</v>
-      </c>
-      <c r="CY1" t="str">
-        <f t="shared" si="0"/>
-        <v>10010100</v>
-      </c>
-      <c r="CZ1" t="str">
-        <f t="shared" si="0"/>
-        <v>01100011</v>
-      </c>
-      <c r="DA1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
-      </c>
-      <c r="DB1" t="str">
-        <f t="shared" si="0"/>
-        <v>11111111</v>
-      </c>
-      <c r="DC1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000001</v>
-      </c>
-      <c r="DD1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000001</v>
-      </c>
-      <c r="DE1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000001</v>
-      </c>
-      <c r="DF1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
-      </c>
-      <c r="DG1" t="str">
-        <f t="shared" si="0"/>
-        <v>11111111</v>
-      </c>
-      <c r="DH1" t="str">
-        <f t="shared" si="0"/>
-        <v>10000001</v>
-      </c>
-      <c r="DI1" t="str">
-        <f t="shared" ref="DI1" si="1">LEN(BB1)&amp;LEN(BB2)&amp;LEN(BB3)&amp;LEN(BB4)&amp;LEN(BB5)&amp;LEN(BB6)&amp;LEN(BB7)&amp;LEN(BB8)</f>
-        <v>01000010</v>
-      </c>
-      <c r="DJ1" t="str">
-        <f t="shared" ref="DJ1" si="2">LEN(BC1)&amp;LEN(BC2)&amp;LEN(BC3)&amp;LEN(BC4)&amp;LEN(BC5)&amp;LEN(BC6)&amp;LEN(BC7)&amp;LEN(BC8)</f>
-        <v>00111100</v>
-      </c>
-      <c r="DK1" t="str">
-        <f t="shared" ref="DK1" si="3">LEN(BD1)&amp;LEN(BD2)&amp;LEN(BD3)&amp;LEN(BD4)&amp;LEN(BD5)&amp;LEN(BD6)&amp;LEN(BD7)&amp;LEN(BD8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="DL1" t="str">
-        <f t="shared" ref="DL1" si="4">LEN(BE1)&amp;LEN(BE2)&amp;LEN(BE3)&amp;LEN(BE4)&amp;LEN(BE5)&amp;LEN(BE6)&amp;LEN(BE7)&amp;LEN(BE8)</f>
-        <v>11111001</v>
-      </c>
-      <c r="DM1" t="str">
-        <f t="shared" ref="DM1" si="5">LEN(BF1)&amp;LEN(BF2)&amp;LEN(BF3)&amp;LEN(BF4)&amp;LEN(BF5)&amp;LEN(BF6)&amp;LEN(BF7)&amp;LEN(BF8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:117" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1791,267 +1776,252 @@
       <c r="AE2" t="s">
         <v>0</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AH2" t="s">
         <v>0</v>
       </c>
       <c r="AK2" t="s">
         <v>0</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AM2" t="s">
         <v>0</v>
       </c>
       <c r="AP2" t="s">
         <v>0</v>
       </c>
-      <c r="AS2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ2" t="s">
+      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
         <v>0</v>
       </c>
       <c r="BB2" t="s">
         <v>0</v>
       </c>
-      <c r="BE2" t="s">
-        <v>0</v>
+      <c r="BG2" t="str">
+        <f>"0x"&amp;BIN2HEX(BG1,2)</f>
+        <v>0xFF</v>
       </c>
       <c r="BH2" t="str">
-        <f>"0x"&amp;BIN2HEX(BH1,2)</f>
+        <f t="shared" ref="BH2:CN2" si="0">"0x"&amp;BIN2HEX(BH1,2)</f>
+        <v>0x18</v>
+      </c>
+      <c r="BI2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x18</v>
+      </c>
+      <c r="BJ2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x18</v>
+      </c>
+      <c r="BK2" t="str">
+        <f t="shared" si="0"/>
         <v>0xFF</v>
       </c>
-      <c r="BI2" t="str">
-        <f t="shared" ref="BI2:CO2" si="6">"0x"&amp;BIN2HEX(BI1,2)</f>
-        <v>0x18</v>
-      </c>
-      <c r="BJ2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x18</v>
-      </c>
-      <c r="BK2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x18</v>
-      </c>
       <c r="BL2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
+        <v>0x00</v>
+      </c>
+      <c r="BM2" t="str">
+        <f t="shared" si="0"/>
         <v>0xFF</v>
       </c>
-      <c r="BM2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BN2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x89</v>
+      </c>
+      <c r="BO2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x89</v>
+      </c>
+      <c r="BP2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x89</v>
+      </c>
+      <c r="BQ2" t="str">
+        <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
-      <c r="BN2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BR2" t="str">
+        <f t="shared" si="0"/>
         <v>0xFF</v>
       </c>
-      <c r="BO2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x89</v>
-      </c>
-      <c r="BP2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x89</v>
-      </c>
-      <c r="BQ2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x89</v>
-      </c>
-      <c r="BR2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BS2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x01</v>
+      </c>
+      <c r="BT2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x01</v>
+      </c>
+      <c r="BU2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x01</v>
+      </c>
+      <c r="BV2" t="str">
+        <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
-      <c r="BS2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BW2" t="str">
+        <f t="shared" si="0"/>
         <v>0xFF</v>
       </c>
-      <c r="BT2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BX2" t="str">
+        <f t="shared" si="0"/>
         <v>0x01</v>
       </c>
-      <c r="BU2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BY2" t="str">
+        <f t="shared" si="0"/>
         <v>0x01</v>
       </c>
-      <c r="BV2" t="str">
-        <f t="shared" si="6"/>
+      <c r="BZ2" t="str">
+        <f t="shared" si="0"/>
         <v>0x01</v>
       </c>
-      <c r="BW2" t="str">
-        <f t="shared" si="6"/>
+      <c r="CA2" t="str">
+        <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
-      <c r="BX2" t="str">
-        <f t="shared" si="6"/>
+      <c r="CB2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x7E</v>
+      </c>
+      <c r="CC2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x81</v>
+      </c>
+      <c r="CD2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x81</v>
+      </c>
+      <c r="CE2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x7E</v>
+      </c>
+      <c r="CF2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00</v>
+      </c>
+      <c r="CG2" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFE</v>
+      </c>
+      <c r="CH2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x01</v>
+      </c>
+      <c r="CI2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0E</v>
+      </c>
+      <c r="CJ2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x01</v>
+      </c>
+      <c r="CK2" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFE</v>
+      </c>
+      <c r="CL2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00</v>
+      </c>
+      <c r="CM2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00</v>
+      </c>
+      <c r="CN2" t="str">
+        <f t="shared" si="0"/>
+        <v>0x7E</v>
+      </c>
+      <c r="CO2" t="str">
+        <f t="shared" ref="CO2" si="1">"0x"&amp;BIN2HEX(CO1,2)</f>
+        <v>0x81</v>
+      </c>
+      <c r="CP2" t="str">
+        <f t="shared" ref="CP2" si="2">"0x"&amp;BIN2HEX(CP1,2)</f>
+        <v>0x81</v>
+      </c>
+      <c r="CQ2" t="str">
+        <f t="shared" ref="CQ2" si="3">"0x"&amp;BIN2HEX(CQ1,2)</f>
+        <v>0x7E</v>
+      </c>
+      <c r="CR2" t="str">
+        <f t="shared" ref="CR2" si="4">"0x"&amp;BIN2HEX(CR1,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="CS2" t="str">
+        <f t="shared" ref="CS2" si="5">"0x"&amp;BIN2HEX(CS1,2)</f>
         <v>0xFF</v>
       </c>
-      <c r="BY2" t="str">
-        <f t="shared" si="6"/>
+      <c r="CT2" t="str">
+        <f t="shared" ref="CT2" si="6">"0x"&amp;BIN2HEX(CT1,2)</f>
+        <v>0x98</v>
+      </c>
+      <c r="CU2" t="str">
+        <f t="shared" ref="CU2" si="7">"0x"&amp;BIN2HEX(CU1,2)</f>
+        <v>0x94</v>
+      </c>
+      <c r="CV2" t="str">
+        <f t="shared" ref="CV2" si="8">"0x"&amp;BIN2HEX(CV1,2)</f>
+        <v>0x63</v>
+      </c>
+      <c r="CW2" t="str">
+        <f t="shared" ref="CW2" si="9">"0x"&amp;BIN2HEX(CW1,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="CX2" t="str">
+        <f t="shared" ref="CX2" si="10">"0x"&amp;BIN2HEX(CX1,2)</f>
+        <v>0xFF</v>
+      </c>
+      <c r="CY2" t="str">
+        <f t="shared" ref="CY2" si="11">"0x"&amp;BIN2HEX(CY1,2)</f>
         <v>0x01</v>
       </c>
-      <c r="BZ2" t="str">
-        <f t="shared" si="6"/>
+      <c r="CZ2" t="str">
+        <f t="shared" ref="CZ2" si="12">"0x"&amp;BIN2HEX(CZ1,2)</f>
         <v>0x01</v>
       </c>
-      <c r="CA2" t="str">
-        <f t="shared" si="6"/>
+      <c r="DA2" t="str">
+        <f t="shared" ref="DA2" si="13">"0x"&amp;BIN2HEX(DA1,2)</f>
         <v>0x01</v>
       </c>
-      <c r="CB2" t="str">
-        <f t="shared" si="6"/>
+      <c r="DB2" t="str">
+        <f t="shared" ref="DB2:DG2" si="14">"0x"&amp;BIN2HEX(DB1,2)</f>
         <v>0x00</v>
       </c>
-      <c r="CC2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x7E</v>
-      </c>
-      <c r="CD2" t="str">
-        <f t="shared" si="6"/>
+      <c r="DC2" t="str">
+        <f t="shared" si="14"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DD2" t="str">
+        <f t="shared" si="14"/>
         <v>0x81</v>
       </c>
-      <c r="CE2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x81</v>
-      </c>
-      <c r="CF2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x7E</v>
-      </c>
-      <c r="CG2" t="str">
-        <f t="shared" si="6"/>
+      <c r="DE2" t="str">
+        <f t="shared" si="14"/>
+        <v>0x42</v>
+      </c>
+      <c r="DF2" t="str">
+        <f t="shared" si="14"/>
+        <v>0x3C</v>
+      </c>
+      <c r="DG2" t="str">
+        <f t="shared" si="14"/>
         <v>0x00</v>
       </c>
-      <c r="CH2" t="str">
-        <f t="shared" si="6"/>
-        <v>0xE0</v>
-      </c>
-      <c r="CI2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x1E</v>
-      </c>
-      <c r="CJ2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x01</v>
-      </c>
-      <c r="CK2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x1E</v>
-      </c>
-      <c r="CL2" t="str">
-        <f t="shared" si="6"/>
-        <v>0xE0</v>
-      </c>
-      <c r="CM2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x1E</v>
-      </c>
-      <c r="CN2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x01</v>
-      </c>
-      <c r="CO2" t="str">
-        <f t="shared" si="6"/>
-        <v>0x1E</v>
-      </c>
-      <c r="CP2" t="str">
-        <f t="shared" ref="CP2" si="7">"0x"&amp;BIN2HEX(CP1,2)</f>
-        <v>0xE0</v>
-      </c>
-      <c r="CQ2" t="str">
-        <f t="shared" ref="CQ2" si="8">"0x"&amp;BIN2HEX(CQ1,2)</f>
+      <c r="DH2" t="str">
+        <f t="shared" ref="DH2" si="15">"0x"&amp;BIN2HEX(DH1,2)</f>
+        <v>0xF9</v>
+      </c>
+      <c r="DI2" t="str">
+        <f t="shared" ref="DI2" si="16">"0x"&amp;BIN2HEX(DI1,2)</f>
         <v>0x00</v>
       </c>
-      <c r="CR2" t="str">
-        <f t="shared" ref="CR2" si="9">"0x"&amp;BIN2HEX(CR1,2)</f>
-        <v>0x7E</v>
-      </c>
-      <c r="CS2" t="str">
-        <f t="shared" ref="CS2" si="10">"0x"&amp;BIN2HEX(CS1,2)</f>
-        <v>0x81</v>
-      </c>
-      <c r="CT2" t="str">
-        <f t="shared" ref="CT2" si="11">"0x"&amp;BIN2HEX(CT1,2)</f>
-        <v>0x81</v>
-      </c>
-      <c r="CU2" t="str">
-        <f t="shared" ref="CU2" si="12">"0x"&amp;BIN2HEX(CU1,2)</f>
-        <v>0x7E</v>
-      </c>
-      <c r="CV2" t="str">
-        <f t="shared" ref="CV2" si="13">"0x"&amp;BIN2HEX(CV1,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="CW2" t="str">
-        <f t="shared" ref="CW2" si="14">"0x"&amp;BIN2HEX(CW1,2)</f>
-        <v>0xFF</v>
-      </c>
-      <c r="CX2" t="str">
-        <f t="shared" ref="CX2" si="15">"0x"&amp;BIN2HEX(CX1,2)</f>
-        <v>0x98</v>
-      </c>
-      <c r="CY2" t="str">
-        <f t="shared" ref="CY2" si="16">"0x"&amp;BIN2HEX(CY1,2)</f>
-        <v>0x94</v>
-      </c>
-      <c r="CZ2" t="str">
-        <f t="shared" ref="CZ2" si="17">"0x"&amp;BIN2HEX(CZ1,2)</f>
-        <v>0x63</v>
-      </c>
-      <c r="DA2" t="str">
-        <f t="shared" ref="DA2" si="18">"0x"&amp;BIN2HEX(DA1,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="DB2" t="str">
-        <f t="shared" ref="DB2" si="19">"0x"&amp;BIN2HEX(DB1,2)</f>
-        <v>0xFF</v>
-      </c>
-      <c r="DC2" t="str">
-        <f t="shared" ref="DC2:DH2" si="20">"0x"&amp;BIN2HEX(DC1,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="DD2" t="str">
-        <f t="shared" si="20"/>
-        <v>0x01</v>
-      </c>
-      <c r="DE2" t="str">
-        <f t="shared" si="20"/>
-        <v>0x01</v>
-      </c>
-      <c r="DF2" t="str">
-        <f t="shared" si="20"/>
-        <v>0x00</v>
-      </c>
-      <c r="DG2" t="str">
-        <f t="shared" si="20"/>
-        <v>0xFF</v>
-      </c>
-      <c r="DH2" t="str">
-        <f t="shared" si="20"/>
-        <v>0x81</v>
-      </c>
-      <c r="DI2" t="str">
-        <f t="shared" ref="DI2" si="21">"0x"&amp;BIN2HEX(DI1,2)</f>
-        <v>0x42</v>
-      </c>
-      <c r="DJ2" t="str">
-        <f t="shared" ref="DJ2" si="22">"0x"&amp;BIN2HEX(DJ1,2)</f>
-        <v>0x3C</v>
-      </c>
-      <c r="DK2" t="str">
-        <f t="shared" ref="DK2" si="23">"0x"&amp;BIN2HEX(DK1,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="DL2" t="str">
-        <f t="shared" ref="DL2" si="24">"0x"&amp;BIN2HEX(DL1,2)</f>
-        <v>0xF9</v>
-      </c>
-      <c r="DM2" t="str">
-        <f t="shared" ref="DM2" si="25">"0x"&amp;BIN2HEX(DM1,2)</f>
-        <v>0x00</v>
-      </c>
-    </row>
-    <row r="3" spans="1:117" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2079,35 +2049,32 @@
       <c r="AE3" t="s">
         <v>0</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AH3" t="s">
         <v>0</v>
       </c>
       <c r="AK3" t="s">
         <v>0</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AM3" t="s">
         <v>0</v>
       </c>
       <c r="AP3" t="s">
         <v>0</v>
       </c>
-      <c r="AS3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="s">
+      <c r="AR3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="s">
         <v>0</v>
       </c>
       <c r="AZ3" t="s">
         <v>0</v>
       </c>
-      <c r="BC3" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="BB3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2138,13 +2105,10 @@
       <c r="Y4" t="s">
         <v>0</v>
       </c>
-      <c r="AB4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="s">
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="s">
         <v>0</v>
       </c>
       <c r="AH4" t="s">
@@ -2153,32 +2117,29 @@
       <c r="AK4" t="s">
         <v>0</v>
       </c>
+      <c r="AM4" t="s">
+        <v>0</v>
+      </c>
       <c r="AN4" t="s">
         <v>0</v>
       </c>
-      <c r="AP4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AO4" t="s">
         <v>0</v>
       </c>
       <c r="AR4" t="s">
         <v>0</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AW4" t="s">
         <v>0</v>
       </c>
       <c r="AZ4" t="s">
         <v>0</v>
       </c>
-      <c r="BC4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="BB4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2218,13 +2179,13 @@
       <c r="Y5" t="s">
         <v>0</v>
       </c>
-      <c r="AB5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="s">
+      <c r="AA5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="s">
         <v>0</v>
       </c>
       <c r="AH5" t="s">
@@ -2233,29 +2194,26 @@
       <c r="AK5" t="s">
         <v>0</v>
       </c>
+      <c r="AM5" t="s">
+        <v>0</v>
+      </c>
       <c r="AN5" t="s">
         <v>0</v>
       </c>
-      <c r="AP5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="s">
+      <c r="AR5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
         <v>0</v>
       </c>
       <c r="AZ5" t="s">
         <v>0</v>
       </c>
-      <c r="BC5" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="BB5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2277,13 +2235,13 @@
       <c r="Y6" t="s">
         <v>0</v>
       </c>
-      <c r="AB6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="AA6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
         <v>0</v>
       </c>
       <c r="AH6" t="s">
@@ -2292,26 +2250,23 @@
       <c r="AK6" t="s">
         <v>0</v>
       </c>
-      <c r="AN6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP6" t="s">
+      <c r="AM6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="s">
         <v>0</v>
       </c>
       <c r="AR6" t="s">
         <v>0</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AW6" t="s">
         <v>0</v>
       </c>
       <c r="AZ6" t="s">
         <v>0</v>
       </c>
-      <c r="BC6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:117" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2333,13 +2288,13 @@
       <c r="Y7" t="s">
         <v>0</v>
       </c>
-      <c r="AB7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="s">
+      <c r="AA7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="s">
         <v>0</v>
       </c>
       <c r="AH7" t="s">
@@ -2348,29 +2303,26 @@
       <c r="AK7" t="s">
         <v>0</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AM7" t="s">
         <v>0</v>
       </c>
       <c r="AP7" t="s">
         <v>0</v>
       </c>
-      <c r="AS7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>0</v>
-      </c>
-      <c r="BI7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="AR7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2419,13 +2371,16 @@
       <c r="X8" t="s">
         <v>0</v>
       </c>
-      <c r="AC8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="s">
+      <c r="AB8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>0</v>
       </c>
       <c r="AM8" t="s">
@@ -2434,39 +2389,36 @@
       <c r="AP8" t="s">
         <v>0</v>
       </c>
+      <c r="AR8" t="s">
+        <v>0</v>
+      </c>
       <c r="AS8" t="s">
         <v>0</v>
       </c>
+      <c r="AT8" t="s">
+        <v>0</v>
+      </c>
       <c r="AU8" t="s">
         <v>0</v>
       </c>
-      <c r="AV8" t="s">
-        <v>0</v>
-      </c>
       <c r="AW8" t="s">
         <v>0</v>
       </c>
       <c r="AX8" t="s">
         <v>0</v>
       </c>
-      <c r="AZ8" t="s">
-        <v>0</v>
-      </c>
-      <c r="BA8" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE8" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH8" t="s">
+      <c r="BB8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG8" t="s">
         <v>17</v>
       </c>
-      <c r="BI8" t="str">
-        <f>BI7&amp;BH8&amp;","</f>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="BH8" t="str">
+        <f>BH7&amp;BG8&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2632,33 +2584,24 @@
       <c r="BC9" t="s">
         <v>1</v>
       </c>
-      <c r="BD9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BF9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH9" t="s">
+      <c r="BG9" t="s">
         <v>2</v>
       </c>
-      <c r="BI9" t="str">
-        <f>BI8&amp;" "&amp;BH9&amp;","</f>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH10" t="s">
+      <c r="BH9" t="str">
+        <f>BH8&amp;" "&amp;BG9&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG10" t="s">
         <v>2</v>
       </c>
-      <c r="BI10" t="str">
-        <f t="shared" ref="BI10:BI65" si="26">BI9&amp;" "&amp;BH10&amp;","</f>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:117" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="BH10" t="str">
+        <f t="shared" ref="BH10:BH65" si="17">BH9&amp;" "&amp;BG10&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:113" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -2824,507 +2767,471 @@
       <c r="BC11" s="2">
         <v>55</v>
       </c>
-      <c r="BD11" s="2">
-        <v>56</v>
-      </c>
-      <c r="BE11" s="2">
-        <v>57</v>
-      </c>
-      <c r="BF11" s="2">
-        <v>58</v>
-      </c>
-      <c r="BH11" t="s">
+      <c r="BG11" t="s">
         <v>2</v>
       </c>
-      <c r="BI11" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH12" t="s">
+      <c r="BH11" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG12" t="s">
         <v>17</v>
       </c>
-      <c r="BI12" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH13" t="s">
+      <c r="BH12" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG13" t="s">
         <v>6</v>
       </c>
-      <c r="BI13" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH14" t="s">
+      <c r="BH13" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG14" t="s">
         <v>17</v>
       </c>
-      <c r="BI14" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH15" t="s">
+      <c r="BH14" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG15" t="s">
         <v>18</v>
       </c>
-      <c r="BI15" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="BH16" t="s">
+      <c r="BH15" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="BG16" t="s">
         <v>18</v>
       </c>
-      <c r="BI16" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89,</v>
-      </c>
-    </row>
-    <row r="17" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH17" t="s">
+      <c r="BH16" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="17" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG17" t="s">
         <v>18</v>
       </c>
-      <c r="BI17" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89,</v>
-      </c>
-    </row>
-    <row r="18" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH18" t="s">
+      <c r="BH17" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="18" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG18" t="s">
         <v>6</v>
       </c>
-      <c r="BI18" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00,</v>
-      </c>
-    </row>
-    <row r="19" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH19" t="s">
+      <c r="BH18" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00,</v>
+      </c>
+    </row>
+    <row r="19" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG19" t="s">
         <v>17</v>
       </c>
-      <c r="BI19" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="20" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH20" t="s">
+      <c r="BH19" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="20" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG20" t="s">
         <v>19</v>
       </c>
-      <c r="BI20" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01,</v>
-      </c>
-    </row>
-    <row r="21" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH21" t="s">
+      <c r="BH20" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01,</v>
+      </c>
+    </row>
+    <row r="21" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG21" t="s">
         <v>19</v>
       </c>
-      <c r="BI21" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="22" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH22" t="s">
+      <c r="BH21" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="22" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG22" t="s">
         <v>19</v>
       </c>
-      <c r="BI22" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="23" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH23" t="s">
+      <c r="BH22" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="23" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG23" t="s">
         <v>6</v>
       </c>
-      <c r="BI23" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
-      </c>
-    </row>
-    <row r="24" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH24" t="s">
+      <c r="BH23" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
+      </c>
+    </row>
+    <row r="24" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG24" t="s">
         <v>17</v>
       </c>
-      <c r="BI24" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="25" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH25" t="s">
+      <c r="BH24" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="25" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG25" t="s">
         <v>19</v>
       </c>
-      <c r="BI25" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01,</v>
-      </c>
-    </row>
-    <row r="26" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH26" t="s">
+      <c r="BH25" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01,</v>
+      </c>
+    </row>
+    <row r="26" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG26" t="s">
         <v>19</v>
       </c>
-      <c r="BI26" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="27" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH27" t="s">
+      <c r="BH26" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="27" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG27" t="s">
         <v>19</v>
       </c>
-      <c r="BI27" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="28" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH28" t="s">
+      <c r="BH27" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="28" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG28" t="s">
         <v>6</v>
       </c>
-      <c r="BI28" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
-      </c>
-    </row>
-    <row r="29" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH29" t="s">
+      <c r="BH28" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
+      </c>
+    </row>
+    <row r="29" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG29" t="s">
         <v>20</v>
       </c>
-      <c r="BI29" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E,</v>
-      </c>
-    </row>
-    <row r="30" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH30" t="s">
+      <c r="BH29" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E,</v>
+      </c>
+    </row>
+    <row r="30" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG30" t="s">
         <v>5</v>
       </c>
-      <c r="BI30" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81,</v>
-      </c>
-    </row>
-    <row r="31" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH31" t="s">
+      <c r="BH30" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81,</v>
+      </c>
+    </row>
+    <row r="31" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG31" t="s">
         <v>5</v>
       </c>
-      <c r="BI31" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81,</v>
-      </c>
-    </row>
-    <row r="32" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH32" t="s">
+      <c r="BH31" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81,</v>
+      </c>
+    </row>
+    <row r="32" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG32" t="s">
         <v>20</v>
       </c>
-      <c r="BI32" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
-      </c>
-    </row>
-    <row r="33" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH33" t="s">
+      <c r="BH32" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
+      </c>
+    </row>
+    <row r="33" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG33" t="s">
         <v>6</v>
       </c>
-      <c r="BI33" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
-      </c>
-    </row>
-    <row r="34" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH34" t="s">
+      <c r="BH33" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
+      </c>
+    </row>
+    <row r="34" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH34" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE,</v>
+      </c>
+    </row>
+    <row r="35" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG35" t="s">
+        <v>19</v>
+      </c>
+      <c r="BH35" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01,</v>
+      </c>
+    </row>
+    <row r="36" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG36" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH36" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E,</v>
+      </c>
+    </row>
+    <row r="37" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG37" t="s">
+        <v>19</v>
+      </c>
+      <c r="BH37" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01,</v>
+      </c>
+    </row>
+    <row r="38" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG38" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH38" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE,</v>
+      </c>
+    </row>
+    <row r="39" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG39" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH39" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00,</v>
+      </c>
+    </row>
+    <row r="40" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG40" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH40" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="41" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG41" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH41" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E,</v>
+      </c>
+    </row>
+    <row r="42" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG42" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH42" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81,</v>
+      </c>
+    </row>
+    <row r="43" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG43" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH43" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81,</v>
+      </c>
+    </row>
+    <row r="44" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG44" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH44" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
+      </c>
+    </row>
+    <row r="45" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG45" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
+      </c>
+    </row>
+    <row r="46" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG46" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH46" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="47" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG47" t="s">
         <v>21</v>
       </c>
-      <c r="BI34" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0,</v>
-      </c>
-    </row>
-    <row r="35" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH35" t="s">
+      <c r="BH47" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98,</v>
+      </c>
+    </row>
+    <row r="48" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG48" t="s">
         <v>22</v>
       </c>
-      <c r="BI35" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E,</v>
-      </c>
-    </row>
-    <row r="36" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH36" t="s">
+      <c r="BH48" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94,</v>
+      </c>
+    </row>
+    <row r="49" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG49" t="s">
+        <v>23</v>
+      </c>
+      <c r="BH49" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63,</v>
+      </c>
+    </row>
+    <row r="50" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG50" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH50" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00,</v>
+      </c>
+    </row>
+    <row r="51" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG51" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH51" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="52" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG52" t="s">
         <v>19</v>
       </c>
-      <c r="BI36" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01,</v>
-      </c>
-    </row>
-    <row r="37" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH37" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI37" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E,</v>
-      </c>
-    </row>
-    <row r="38" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH38" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI38" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0,</v>
-      </c>
-    </row>
-    <row r="39" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH39" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI39" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E,</v>
-      </c>
-    </row>
-    <row r="40" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH40" t="s">
+      <c r="BH52" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01,</v>
+      </c>
+    </row>
+    <row r="53" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG53" t="s">
         <v>19</v>
       </c>
-      <c r="BI40" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01,</v>
-      </c>
-    </row>
-    <row r="41" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH41" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI41" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E,</v>
-      </c>
-    </row>
-    <row r="42" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH42" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI42" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0,</v>
-      </c>
-    </row>
-    <row r="43" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH43" t="s">
+      <c r="BH53" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="54" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG54" t="s">
+        <v>19</v>
+      </c>
+      <c r="BH54" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="55" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG55" t="s">
         <v>6</v>
       </c>
-      <c r="BI43" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00,</v>
-      </c>
-    </row>
-    <row r="44" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH44" t="s">
-        <v>20</v>
-      </c>
-      <c r="BI44" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E,</v>
-      </c>
-    </row>
-    <row r="45" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH45" t="s">
+      <c r="BH55" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
+      </c>
+    </row>
+    <row r="56" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG56" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH56" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="57" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG57" t="s">
         <v>5</v>
       </c>
-      <c r="BI45" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81,</v>
-      </c>
-    </row>
-    <row r="46" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH46" t="s">
-        <v>5</v>
-      </c>
-      <c r="BI46" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81,</v>
-      </c>
-    </row>
-    <row r="47" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH47" t="s">
-        <v>20</v>
-      </c>
-      <c r="BI47" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
-      </c>
-    </row>
-    <row r="48" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH48" t="s">
+      <c r="BH57" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81,</v>
+      </c>
+    </row>
+    <row r="58" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG58" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH58" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42,</v>
+      </c>
+    </row>
+    <row r="59" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG59" t="s">
+        <v>24</v>
+      </c>
+      <c r="BH59" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C,</v>
+      </c>
+    </row>
+    <row r="60" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG60" t="s">
         <v>6</v>
       </c>
-      <c r="BI48" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
-      </c>
-    </row>
-    <row r="49" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH49" t="s">
-        <v>17</v>
-      </c>
-      <c r="BI49" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="50" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH50" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI50" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98,</v>
-      </c>
-    </row>
-    <row r="51" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH51" t="s">
-        <v>24</v>
-      </c>
-      <c r="BI51" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94,</v>
-      </c>
-    </row>
-    <row r="52" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH52" t="s">
+      <c r="BH60" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00,</v>
+      </c>
+    </row>
+    <row r="61" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG61" t="s">
         <v>25</v>
       </c>
-      <c r="BI52" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63,</v>
-      </c>
-    </row>
-    <row r="53" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH53" t="s">
+      <c r="BH61" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9,</v>
+      </c>
+    </row>
+    <row r="62" spans="59:60" x14ac:dyDescent="0.25">
+      <c r="BG62" t="s">
         <v>6</v>
       </c>
-      <c r="BI53" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00,</v>
-      </c>
-    </row>
-    <row r="54" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH54" t="s">
-        <v>17</v>
-      </c>
-      <c r="BI54" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="55" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH55" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI55" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01,</v>
-      </c>
-    </row>
-    <row r="56" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH56" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI56" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="57" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH57" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI57" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
-      </c>
-    </row>
-    <row r="58" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH58" t="s">
-        <v>6</v>
-      </c>
-      <c r="BI58" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
-      </c>
-    </row>
-    <row r="59" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH59" t="s">
-        <v>17</v>
-      </c>
-      <c r="BI59" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
-      </c>
-    </row>
-    <row r="60" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH60" t="s">
-        <v>5</v>
-      </c>
-      <c r="BI60" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81,</v>
-      </c>
-    </row>
-    <row r="61" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH61" t="s">
-        <v>4</v>
-      </c>
-      <c r="BI61" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42,</v>
-      </c>
-    </row>
-    <row r="62" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH62" t="s">
-        <v>26</v>
-      </c>
-      <c r="BI62" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C,</v>
-      </c>
-    </row>
-    <row r="63" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH63" t="s">
-        <v>6</v>
-      </c>
-      <c r="BI63" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00,</v>
-      </c>
-    </row>
-    <row r="64" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH64" t="s">
-        <v>27</v>
-      </c>
-      <c r="BI64" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9,</v>
-      </c>
-    </row>
-    <row r="65" spans="60:61" x14ac:dyDescent="0.25">
-      <c r="BH65" t="s">
-        <v>6</v>
-      </c>
-      <c r="BI65" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[HELLO_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x1E, 0x01, 0x1E, 0xE0, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00,</v>
+      <c r="BH62" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Whirled Peas pattern
</commit_message>
<xml_diff>
--- a/02_PersistenceOfVision/Pattern_Calcs.xlsx
+++ b/02_PersistenceOfVision/Pattern_Calcs.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410AF400-BDD4-4078-92C1-6E291A081F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C7BAD9-01A8-4CD4-8C99-CC94002F4E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="5790" windowWidth="24555" windowHeight="13305" xr2:uid="{4F6297C5-B3B5-48D5-ADDF-AF5E88E5519F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{4F6297C5-B3B5-48D5-ADDF-AF5E88E5519F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ovals" sheetId="1" r:id="rId1"/>
     <sheet name="Hello" sheetId="2" r:id="rId2"/>
+    <sheet name="WhirledPeas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="31">
   <si>
     <t>X</t>
   </si>
@@ -93,6 +94,27 @@
   </si>
   <si>
     <t>0x50</t>
+  </si>
+  <si>
+    <t>0x90</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>0x1F</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>0x88</t>
+  </si>
+  <si>
+    <t>0x72</t>
+  </si>
+  <si>
+    <t>0x46</t>
   </si>
 </sst>
 </file>
@@ -452,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D9FD55-98F9-4555-8D5E-2E6E031A5166}">
   <dimension ref="A1:DA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AZ11" sqref="AZ11"/>
     </sheetView>
   </sheetViews>
@@ -498,7 +520,7 @@
         <v>00011000</v>
       </c>
       <c r="BC1" t="str">
-        <f t="shared" ref="BC1:CI1" si="0">LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
+        <f t="shared" ref="BC1:CH1" si="0">LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
         <v>00100100</v>
       </c>
       <c r="BD1" t="str">
@@ -630,7 +652,7 @@
         <v>00000000</v>
       </c>
       <c r="CJ1" t="str">
-        <f t="shared" ref="CJ1:DB1" si="1">LEN(AI1)&amp;LEN(AI2)&amp;LEN(AI3)&amp;LEN(AI4)&amp;LEN(AI5)&amp;LEN(AI6)&amp;LEN(AI7)&amp;LEN(AI8)</f>
+        <f t="shared" ref="CJ1:DA1" si="1">LEN(AI1)&amp;LEN(AI2)&amp;LEN(AI3)&amp;LEN(AI4)&amp;LEN(AI5)&amp;LEN(AI6)&amp;LEN(AI7)&amp;LEN(AI8)</f>
         <v>00000000</v>
       </c>
       <c r="CK1" t="str">
@@ -855,7 +877,7 @@
         <v>0x00</v>
       </c>
       <c r="CJ2" t="str">
-        <f t="shared" ref="CJ2:DB2" si="3">"0x"&amp;BIN2HEX(CJ1,2)</f>
+        <f t="shared" ref="CJ2:DA2" si="3">"0x"&amp;BIN2HEX(CJ1,2)</f>
         <v>0x00</v>
       </c>
       <c r="CK2" t="str">
@@ -1850,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AAAADA-9358-4C28-B2E0-ECDDA6F974A8}">
   <dimension ref="A1:EM77"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="BU1" sqref="BU1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,10 +1919,13 @@
       <c r="AM1" t="s">
         <v>0</v>
       </c>
+      <c r="AP1" t="s">
+        <v>0</v>
+      </c>
       <c r="AQ1" t="s">
         <v>0</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>0</v>
       </c>
       <c r="AU1" t="s">
@@ -1909,295 +1934,292 @@
       <c r="AV1" t="s">
         <v>0</v>
       </c>
-      <c r="AW1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ1" t="s">
+      <c r="AY1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD1" t="s">
         <v>0</v>
       </c>
       <c r="BE1" t="s">
         <v>0</v>
       </c>
-      <c r="BF1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ1" t="s">
+      <c r="BI1" t="s">
         <v>0</v>
       </c>
       <c r="BV1" t="str">
-        <f>LEN(A1)&amp;LEN(A2)&amp;LEN(A3)&amp;LEN(A4)&amp;LEN(A5)&amp;LEN(A6)&amp;LEN(A7)&amp;LEN(A8)</f>
+        <f t="shared" ref="BV1:DA1" si="0">LEN(A1)&amp;LEN(A2)&amp;LEN(A3)&amp;LEN(A4)&amp;LEN(A5)&amp;LEN(A6)&amp;LEN(A7)&amp;LEN(A8)</f>
         <v>11111111</v>
       </c>
       <c r="BW1" t="str">
-        <f>LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
+        <f t="shared" si="0"/>
         <v>00011000</v>
       </c>
       <c r="BX1" t="str">
-        <f>LEN(C1)&amp;LEN(C2)&amp;LEN(C3)&amp;LEN(C4)&amp;LEN(C5)&amp;LEN(C6)&amp;LEN(C7)&amp;LEN(C8)</f>
+        <f t="shared" si="0"/>
         <v>00011000</v>
       </c>
       <c r="BY1" t="str">
-        <f>LEN(D1)&amp;LEN(D2)&amp;LEN(D3)&amp;LEN(D4)&amp;LEN(D5)&amp;LEN(D6)&amp;LEN(D7)&amp;LEN(D8)</f>
+        <f t="shared" si="0"/>
         <v>00011000</v>
       </c>
       <c r="BZ1" t="str">
-        <f>LEN(E1)&amp;LEN(E2)&amp;LEN(E3)&amp;LEN(E4)&amp;LEN(E5)&amp;LEN(E6)&amp;LEN(E7)&amp;LEN(E8)</f>
+        <f t="shared" si="0"/>
         <v>11111111</v>
       </c>
       <c r="CA1" t="str">
-        <f>LEN(F1)&amp;LEN(F2)&amp;LEN(F3)&amp;LEN(F4)&amp;LEN(F5)&amp;LEN(F6)&amp;LEN(F7)&amp;LEN(F8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CB1" t="str">
-        <f>LEN(G1)&amp;LEN(G2)&amp;LEN(G3)&amp;LEN(G4)&amp;LEN(G5)&amp;LEN(G6)&amp;LEN(G7)&amp;LEN(G8)</f>
+        <f t="shared" si="0"/>
         <v>11111111</v>
       </c>
       <c r="CC1" t="str">
-        <f>LEN(H1)&amp;LEN(H2)&amp;LEN(H3)&amp;LEN(H4)&amp;LEN(H5)&amp;LEN(H6)&amp;LEN(H7)&amp;LEN(H8)</f>
+        <f t="shared" si="0"/>
         <v>10001001</v>
       </c>
       <c r="CD1" t="str">
-        <f>LEN(I1)&amp;LEN(I2)&amp;LEN(I3)&amp;LEN(I4)&amp;LEN(I5)&amp;LEN(I6)&amp;LEN(I7)&amp;LEN(I8)</f>
+        <f t="shared" si="0"/>
         <v>10001001</v>
       </c>
       <c r="CE1" t="str">
-        <f>LEN(J1)&amp;LEN(J2)&amp;LEN(J3)&amp;LEN(J4)&amp;LEN(J5)&amp;LEN(J6)&amp;LEN(J7)&amp;LEN(J8)</f>
+        <f t="shared" si="0"/>
         <v>10001001</v>
       </c>
       <c r="CF1" t="str">
-        <f>LEN(K1)&amp;LEN(K2)&amp;LEN(K3)&amp;LEN(K4)&amp;LEN(K5)&amp;LEN(K6)&amp;LEN(K7)&amp;LEN(K8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CG1" t="str">
-        <f>LEN(L1)&amp;LEN(L2)&amp;LEN(L3)&amp;LEN(L4)&amp;LEN(L5)&amp;LEN(L6)&amp;LEN(L7)&amp;LEN(L8)</f>
+        <f t="shared" si="0"/>
         <v>11111111</v>
       </c>
       <c r="CH1" t="str">
-        <f>LEN(M1)&amp;LEN(M2)&amp;LEN(M3)&amp;LEN(M4)&amp;LEN(M5)&amp;LEN(M6)&amp;LEN(M7)&amp;LEN(M8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CI1" t="str">
-        <f>LEN(N1)&amp;LEN(N2)&amp;LEN(N3)&amp;LEN(N4)&amp;LEN(N5)&amp;LEN(N6)&amp;LEN(N7)&amp;LEN(N8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CJ1" t="str">
-        <f>LEN(O1)&amp;LEN(O2)&amp;LEN(O3)&amp;LEN(O4)&amp;LEN(O5)&amp;LEN(O6)&amp;LEN(O7)&amp;LEN(O8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CK1" t="str">
-        <f>LEN(P1)&amp;LEN(P2)&amp;LEN(P3)&amp;LEN(P4)&amp;LEN(P5)&amp;LEN(P6)&amp;LEN(P7)&amp;LEN(P8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CL1" t="str">
-        <f>LEN(Q1)&amp;LEN(Q2)&amp;LEN(Q3)&amp;LEN(Q4)&amp;LEN(Q5)&amp;LEN(Q6)&amp;LEN(Q7)&amp;LEN(Q8)</f>
+        <f t="shared" si="0"/>
         <v>11111111</v>
       </c>
       <c r="CM1" t="str">
-        <f>LEN(R1)&amp;LEN(R2)&amp;LEN(R3)&amp;LEN(R4)&amp;LEN(R5)&amp;LEN(R6)&amp;LEN(R7)&amp;LEN(R8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CN1" t="str">
-        <f>LEN(S1)&amp;LEN(S2)&amp;LEN(S3)&amp;LEN(S4)&amp;LEN(S5)&amp;LEN(S6)&amp;LEN(S7)&amp;LEN(S8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CO1" t="str">
-        <f>LEN(T1)&amp;LEN(T2)&amp;LEN(T3)&amp;LEN(T4)&amp;LEN(T5)&amp;LEN(T6)&amp;LEN(T7)&amp;LEN(T8)</f>
+        <f t="shared" si="0"/>
         <v>00000001</v>
       </c>
       <c r="CP1" t="str">
-        <f>LEN(U1)&amp;LEN(U2)&amp;LEN(U3)&amp;LEN(U4)&amp;LEN(U5)&amp;LEN(U6)&amp;LEN(U7)&amp;LEN(U8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CQ1" t="str">
-        <f>LEN(V1)&amp;LEN(V2)&amp;LEN(V3)&amp;LEN(V4)&amp;LEN(V5)&amp;LEN(V6)&amp;LEN(V7)&amp;LEN(V8)</f>
+        <f t="shared" si="0"/>
         <v>01111110</v>
       </c>
       <c r="CR1" t="str">
-        <f>LEN(W1)&amp;LEN(W2)&amp;LEN(W3)&amp;LEN(W4)&amp;LEN(W5)&amp;LEN(W6)&amp;LEN(W7)&amp;LEN(W8)</f>
+        <f t="shared" si="0"/>
         <v>10000001</v>
       </c>
       <c r="CS1" t="str">
-        <f>LEN(X1)&amp;LEN(X2)&amp;LEN(X3)&amp;LEN(X4)&amp;LEN(X5)&amp;LEN(X6)&amp;LEN(X7)&amp;LEN(X8)</f>
+        <f t="shared" si="0"/>
         <v>10000001</v>
       </c>
       <c r="CT1" t="str">
-        <f>LEN(Y1)&amp;LEN(Y2)&amp;LEN(Y3)&amp;LEN(Y4)&amp;LEN(Y5)&amp;LEN(Y6)&amp;LEN(Y7)&amp;LEN(Y8)</f>
+        <f t="shared" si="0"/>
         <v>01111110</v>
       </c>
       <c r="CU1" t="str">
-        <f>LEN(Z1)&amp;LEN(Z2)&amp;LEN(Z3)&amp;LEN(Z4)&amp;LEN(Z5)&amp;LEN(Z6)&amp;LEN(Z7)&amp;LEN(Z8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CV1" t="str">
-        <f>LEN(AA1)&amp;LEN(AA2)&amp;LEN(AA3)&amp;LEN(AA4)&amp;LEN(AA5)&amp;LEN(AA6)&amp;LEN(AA7)&amp;LEN(AA8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CW1" t="str">
-        <f>LEN(AB1)&amp;LEN(AB2)&amp;LEN(AB3)&amp;LEN(AB4)&amp;LEN(AB5)&amp;LEN(AB6)&amp;LEN(AB7)&amp;LEN(AB8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CX1" t="str">
-        <f>LEN(AC1)&amp;LEN(AC2)&amp;LEN(AC3)&amp;LEN(AC4)&amp;LEN(AC5)&amp;LEN(AC6)&amp;LEN(AC7)&amp;LEN(AC8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CY1" t="str">
-        <f>LEN(AD1)&amp;LEN(AD2)&amp;LEN(AD3)&amp;LEN(AD4)&amp;LEN(AD5)&amp;LEN(AD6)&amp;LEN(AD7)&amp;LEN(AD8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="CZ1" t="str">
-        <f>LEN(AE1)&amp;LEN(AE2)&amp;LEN(AE3)&amp;LEN(AE4)&amp;LEN(AE5)&amp;LEN(AE6)&amp;LEN(AE7)&amp;LEN(AE8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="DA1" t="str">
-        <f>LEN(AF1)&amp;LEN(AF2)&amp;LEN(AF3)&amp;LEN(AF4)&amp;LEN(AF5)&amp;LEN(AF6)&amp;LEN(AF7)&amp;LEN(AF8)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="DB1" t="str">
-        <f>LEN(AG1)&amp;LEN(AG2)&amp;LEN(AG3)&amp;LEN(AG4)&amp;LEN(AG5)&amp;LEN(AG6)&amp;LEN(AG7)&amp;LEN(AG8)</f>
+        <f t="shared" ref="DB1:EG1" si="1">LEN(AG1)&amp;LEN(AG2)&amp;LEN(AG3)&amp;LEN(AG4)&amp;LEN(AG5)&amp;LEN(AG6)&amp;LEN(AG7)&amp;LEN(AG8)</f>
         <v>00000000</v>
       </c>
       <c r="DC1" t="str">
-        <f>LEN(AH1)&amp;LEN(AH2)&amp;LEN(AH3)&amp;LEN(AH4)&amp;LEN(AH5)&amp;LEN(AH6)&amp;LEN(AH7)&amp;LEN(AH8)</f>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="DD1" t="str">
-        <f>LEN(AI1)&amp;LEN(AI2)&amp;LEN(AI3)&amp;LEN(AI4)&amp;LEN(AI5)&amp;LEN(AI6)&amp;LEN(AI7)&amp;LEN(AI8)</f>
+        <f t="shared" si="1"/>
         <v>11111110</v>
       </c>
       <c r="DE1" t="str">
-        <f>LEN(AJ1)&amp;LEN(AJ2)&amp;LEN(AJ3)&amp;LEN(AJ4)&amp;LEN(AJ5)&amp;LEN(AJ6)&amp;LEN(AJ7)&amp;LEN(AJ8)</f>
+        <f t="shared" si="1"/>
         <v>00000001</v>
       </c>
       <c r="DF1" t="str">
-        <f>LEN(AK1)&amp;LEN(AK2)&amp;LEN(AK3)&amp;LEN(AK4)&amp;LEN(AK5)&amp;LEN(AK6)&amp;LEN(AK7)&amp;LEN(AK8)</f>
+        <f t="shared" si="1"/>
         <v>00001110</v>
       </c>
       <c r="DG1" t="str">
-        <f>LEN(AL1)&amp;LEN(AL2)&amp;LEN(AL3)&amp;LEN(AL4)&amp;LEN(AL5)&amp;LEN(AL6)&amp;LEN(AL7)&amp;LEN(AL8)</f>
+        <f t="shared" si="1"/>
         <v>00000001</v>
       </c>
       <c r="DH1" t="str">
-        <f>LEN(AM1)&amp;LEN(AM2)&amp;LEN(AM3)&amp;LEN(AM4)&amp;LEN(AM5)&amp;LEN(AM6)&amp;LEN(AM7)&amp;LEN(AM8)</f>
+        <f t="shared" si="1"/>
         <v>11111110</v>
       </c>
       <c r="DI1" t="str">
-        <f>LEN(AN1)&amp;LEN(AN2)&amp;LEN(AN3)&amp;LEN(AN4)&amp;LEN(AN5)&amp;LEN(AN6)&amp;LEN(AN7)&amp;LEN(AN8)</f>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="DJ1" t="str">
-        <f>LEN(AO1)&amp;LEN(AO2)&amp;LEN(AO3)&amp;LEN(AO4)&amp;LEN(AO5)&amp;LEN(AO6)&amp;LEN(AO7)&amp;LEN(AO8)</f>
-        <v>00000000</v>
+        <f t="shared" si="1"/>
+        <v>01111110</v>
       </c>
       <c r="DK1" t="str">
-        <f>LEN(AP1)&amp;LEN(AP2)&amp;LEN(AP3)&amp;LEN(AP4)&amp;LEN(AP5)&amp;LEN(AP6)&amp;LEN(AP7)&amp;LEN(AP8)</f>
+        <f t="shared" si="1"/>
+        <v>10000001</v>
+      </c>
+      <c r="DL1" t="str">
+        <f t="shared" si="1"/>
+        <v>10000001</v>
+      </c>
+      <c r="DM1" t="str">
+        <f t="shared" si="1"/>
         <v>01111110</v>
       </c>
-      <c r="DL1" t="str">
-        <f>LEN(AQ1)&amp;LEN(AQ2)&amp;LEN(AQ3)&amp;LEN(AQ4)&amp;LEN(AQ5)&amp;LEN(AQ6)&amp;LEN(AQ7)&amp;LEN(AQ8)</f>
+      <c r="DN1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="DO1" t="str">
+        <f t="shared" si="1"/>
+        <v>11111111</v>
+      </c>
+      <c r="DP1" t="str">
+        <f t="shared" si="1"/>
+        <v>10011000</v>
+      </c>
+      <c r="DQ1" t="str">
+        <f t="shared" si="1"/>
+        <v>10010100</v>
+      </c>
+      <c r="DR1" t="str">
+        <f t="shared" si="1"/>
+        <v>01100011</v>
+      </c>
+      <c r="DS1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="DT1" t="str">
+        <f t="shared" si="1"/>
+        <v>11111111</v>
+      </c>
+      <c r="DU1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000001</v>
+      </c>
+      <c r="DV1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000001</v>
+      </c>
+      <c r="DW1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000001</v>
+      </c>
+      <c r="DX1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="DY1" t="str">
+        <f t="shared" ref="DY1:EL1" si="2">LEN(BD1)&amp;LEN(BD2)&amp;LEN(BD3)&amp;LEN(BD4)&amp;LEN(BD5)&amp;LEN(BD6)&amp;LEN(BD7)&amp;LEN(BD8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="DZ1" t="str">
+        <f t="shared" si="2"/>
         <v>10000001</v>
       </c>
-      <c r="DM1" t="str">
-        <f>LEN(AR1)&amp;LEN(AR2)&amp;LEN(AR3)&amp;LEN(AR4)&amp;LEN(AR5)&amp;LEN(AR6)&amp;LEN(AR7)&amp;LEN(AR8)</f>
-        <v>10000001</v>
-      </c>
-      <c r="DN1" t="str">
-        <f>LEN(AS1)&amp;LEN(AS2)&amp;LEN(AS3)&amp;LEN(AS4)&amp;LEN(AS5)&amp;LEN(AS6)&amp;LEN(AS7)&amp;LEN(AS8)</f>
-        <v>01111110</v>
-      </c>
-      <c r="DO1" t="str">
-        <f>LEN(AT1)&amp;LEN(AT2)&amp;LEN(AT3)&amp;LEN(AT4)&amp;LEN(AT5)&amp;LEN(AT6)&amp;LEN(AT7)&amp;LEN(AT8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="DP1" t="str">
-        <f>LEN(AU1)&amp;LEN(AU2)&amp;LEN(AU3)&amp;LEN(AU4)&amp;LEN(AU5)&amp;LEN(AU6)&amp;LEN(AU7)&amp;LEN(AU8)</f>
-        <v>11111111</v>
-      </c>
-      <c r="DQ1" t="str">
-        <f>LEN(AV1)&amp;LEN(AV2)&amp;LEN(AV3)&amp;LEN(AV4)&amp;LEN(AV5)&amp;LEN(AV6)&amp;LEN(AV7)&amp;LEN(AV8)</f>
-        <v>10011000</v>
-      </c>
-      <c r="DR1" t="str">
-        <f>LEN(AW1)&amp;LEN(AW2)&amp;LEN(AW3)&amp;LEN(AW4)&amp;LEN(AW5)&amp;LEN(AW6)&amp;LEN(AW7)&amp;LEN(AW8)</f>
-        <v>10010100</v>
-      </c>
-      <c r="DS1" t="str">
-        <f>LEN(AX1)&amp;LEN(AX2)&amp;LEN(AX3)&amp;LEN(AX4)&amp;LEN(AX5)&amp;LEN(AX6)&amp;LEN(AX7)&amp;LEN(AX8)</f>
-        <v>01100011</v>
-      </c>
-      <c r="DT1" t="str">
-        <f>LEN(AY1)&amp;LEN(AY2)&amp;LEN(AY3)&amp;LEN(AY4)&amp;LEN(AY5)&amp;LEN(AY6)&amp;LEN(AY7)&amp;LEN(AY8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="DU1" t="str">
-        <f>LEN(AZ1)&amp;LEN(AZ2)&amp;LEN(AZ3)&amp;LEN(AZ4)&amp;LEN(AZ5)&amp;LEN(AZ6)&amp;LEN(AZ7)&amp;LEN(AZ8)</f>
-        <v>11111111</v>
-      </c>
-      <c r="DV1" t="str">
-        <f>LEN(BA1)&amp;LEN(BA2)&amp;LEN(BA3)&amp;LEN(BA4)&amp;LEN(BA5)&amp;LEN(BA6)&amp;LEN(BA7)&amp;LEN(BA8)</f>
-        <v>00000001</v>
-      </c>
-      <c r="DW1" t="str">
-        <f>LEN(BB1)&amp;LEN(BB2)&amp;LEN(BB3)&amp;LEN(BB4)&amp;LEN(BB5)&amp;LEN(BB6)&amp;LEN(BB7)&amp;LEN(BB8)</f>
-        <v>00000001</v>
-      </c>
-      <c r="DX1" t="str">
-        <f>LEN(BC1)&amp;LEN(BC2)&amp;LEN(BC3)&amp;LEN(BC4)&amp;LEN(BC5)&amp;LEN(BC6)&amp;LEN(BC7)&amp;LEN(BC8)</f>
-        <v>00000001</v>
-      </c>
-      <c r="DY1" t="str">
-        <f t="shared" ref="DY1:ER1" si="0">LEN(BD1)&amp;LEN(BD2)&amp;LEN(BD3)&amp;LEN(BD4)&amp;LEN(BD5)&amp;LEN(BD6)&amp;LEN(BD7)&amp;LEN(BD8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="DZ1" t="str">
-        <f t="shared" si="0"/>
-        <v>11111111</v>
-      </c>
       <c r="EA1" t="str">
-        <f t="shared" si="0"/>
-        <v>10000001</v>
+        <f t="shared" si="2"/>
+        <v>01000010</v>
       </c>
       <c r="EB1" t="str">
-        <f t="shared" si="0"/>
-        <v>01000010</v>
+        <f t="shared" si="2"/>
+        <v>00111100</v>
       </c>
       <c r="EC1" t="str">
-        <f t="shared" si="0"/>
-        <v>00111100</v>
+        <f t="shared" si="2"/>
+        <v>00000000</v>
       </c>
       <c r="ED1" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
+        <f t="shared" si="2"/>
+        <v>11111001</v>
       </c>
       <c r="EE1" t="str">
-        <f t="shared" si="0"/>
-        <v>11111001</v>
+        <f t="shared" si="2"/>
+        <v>00000000</v>
       </c>
       <c r="EF1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EG1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EH1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EI1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EJ1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EK1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EL1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="EM1" t="str">
@@ -2233,28 +2255,28 @@
       <c r="AM2" t="s">
         <v>0</v>
       </c>
-      <c r="AP2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ2" t="s">
+      <c r="AO2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="s">
         <v>0</v>
       </c>
       <c r="BV2" t="str">
@@ -2262,279 +2284,279 @@
         <v>0xFF</v>
       </c>
       <c r="BW2" t="str">
-        <f t="shared" ref="BW2:DC2" si="1">"0x"&amp;BIN2HEX(BW1,2)</f>
+        <f t="shared" ref="BW2:DC2" si="3">"0x"&amp;BIN2HEX(BW1,2)</f>
         <v>0x18</v>
       </c>
       <c r="BX2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x18</v>
       </c>
       <c r="BY2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x18</v>
       </c>
       <c r="BZ2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0xFF</v>
       </c>
       <c r="CA2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CB2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0xFF</v>
       </c>
       <c r="CC2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x89</v>
       </c>
       <c r="CD2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x89</v>
       </c>
       <c r="CE2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x89</v>
       </c>
       <c r="CF2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CG2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0xFF</v>
       </c>
       <c r="CH2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CI2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CJ2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CK2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CL2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0xFF</v>
       </c>
       <c r="CM2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CN2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CO2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x01</v>
       </c>
       <c r="CP2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CQ2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x7E</v>
       </c>
       <c r="CR2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x81</v>
       </c>
       <c r="CS2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x81</v>
       </c>
       <c r="CT2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x7E</v>
       </c>
       <c r="CU2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CV2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CW2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CX2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CY2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="CZ2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="DA2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="DB2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="DC2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0x00</v>
       </c>
       <c r="DD2" t="str">
-        <f t="shared" ref="DD2" si="2">"0x"&amp;BIN2HEX(DD1,2)</f>
+        <f t="shared" ref="DD2" si="4">"0x"&amp;BIN2HEX(DD1,2)</f>
         <v>0xFE</v>
       </c>
       <c r="DE2" t="str">
-        <f t="shared" ref="DE2" si="3">"0x"&amp;BIN2HEX(DE1,2)</f>
+        <f t="shared" ref="DE2" si="5">"0x"&amp;BIN2HEX(DE1,2)</f>
         <v>0x01</v>
       </c>
       <c r="DF2" t="str">
-        <f t="shared" ref="DF2" si="4">"0x"&amp;BIN2HEX(DF1,2)</f>
+        <f t="shared" ref="DF2" si="6">"0x"&amp;BIN2HEX(DF1,2)</f>
         <v>0x0E</v>
       </c>
       <c r="DG2" t="str">
-        <f t="shared" ref="DG2" si="5">"0x"&amp;BIN2HEX(DG1,2)</f>
+        <f t="shared" ref="DG2" si="7">"0x"&amp;BIN2HEX(DG1,2)</f>
         <v>0x01</v>
       </c>
       <c r="DH2" t="str">
-        <f t="shared" ref="DH2" si="6">"0x"&amp;BIN2HEX(DH1,2)</f>
+        <f t="shared" ref="DH2" si="8">"0x"&amp;BIN2HEX(DH1,2)</f>
         <v>0xFE</v>
       </c>
       <c r="DI2" t="str">
-        <f t="shared" ref="DI2" si="7">"0x"&amp;BIN2HEX(DI1,2)</f>
+        <f t="shared" ref="DI2" si="9">"0x"&amp;BIN2HEX(DI1,2)</f>
         <v>0x00</v>
       </c>
       <c r="DJ2" t="str">
-        <f t="shared" ref="DJ2" si="8">"0x"&amp;BIN2HEX(DJ1,2)</f>
-        <v>0x00</v>
+        <f t="shared" ref="DJ2" si="10">"0x"&amp;BIN2HEX(DJ1,2)</f>
+        <v>0x7E</v>
       </c>
       <c r="DK2" t="str">
-        <f t="shared" ref="DK2" si="9">"0x"&amp;BIN2HEX(DK1,2)</f>
+        <f t="shared" ref="DK2" si="11">"0x"&amp;BIN2HEX(DK1,2)</f>
+        <v>0x81</v>
+      </c>
+      <c r="DL2" t="str">
+        <f t="shared" ref="DL2" si="12">"0x"&amp;BIN2HEX(DL1,2)</f>
+        <v>0x81</v>
+      </c>
+      <c r="DM2" t="str">
+        <f t="shared" ref="DM2" si="13">"0x"&amp;BIN2HEX(DM1,2)</f>
         <v>0x7E</v>
       </c>
-      <c r="DL2" t="str">
-        <f t="shared" ref="DL2" si="10">"0x"&amp;BIN2HEX(DL1,2)</f>
-        <v>0x81</v>
-      </c>
-      <c r="DM2" t="str">
-        <f t="shared" ref="DM2" si="11">"0x"&amp;BIN2HEX(DM1,2)</f>
-        <v>0x81</v>
-      </c>
       <c r="DN2" t="str">
-        <f t="shared" ref="DN2" si="12">"0x"&amp;BIN2HEX(DN1,2)</f>
-        <v>0x7E</v>
+        <f t="shared" ref="DN2" si="14">"0x"&amp;BIN2HEX(DN1,2)</f>
+        <v>0x00</v>
       </c>
       <c r="DO2" t="str">
-        <f t="shared" ref="DO2" si="13">"0x"&amp;BIN2HEX(DO1,2)</f>
-        <v>0x00</v>
+        <f t="shared" ref="DO2" si="15">"0x"&amp;BIN2HEX(DO1,2)</f>
+        <v>0xFF</v>
       </c>
       <c r="DP2" t="str">
-        <f t="shared" ref="DP2" si="14">"0x"&amp;BIN2HEX(DP1,2)</f>
-        <v>0xFF</v>
+        <f t="shared" ref="DP2" si="16">"0x"&amp;BIN2HEX(DP1,2)</f>
+        <v>0x98</v>
       </c>
       <c r="DQ2" t="str">
-        <f t="shared" ref="DQ2:DV2" si="15">"0x"&amp;BIN2HEX(DQ1,2)</f>
-        <v>0x98</v>
+        <f t="shared" ref="DQ2:DV2" si="17">"0x"&amp;BIN2HEX(DQ1,2)</f>
+        <v>0x94</v>
       </c>
       <c r="DR2" t="str">
-        <f t="shared" si="15"/>
-        <v>0x94</v>
+        <f t="shared" si="17"/>
+        <v>0x63</v>
       </c>
       <c r="DS2" t="str">
-        <f t="shared" si="15"/>
-        <v>0x63</v>
+        <f t="shared" si="17"/>
+        <v>0x00</v>
       </c>
       <c r="DT2" t="str">
-        <f t="shared" si="15"/>
-        <v>0x00</v>
-      </c>
-      <c r="DU2" t="str">
-        <f t="shared" si="15"/>
-        <v>0xFF</v>
-      </c>
-      <c r="DV2" t="str">
-        <f t="shared" si="15"/>
-        <v>0x01</v>
-      </c>
-      <c r="DW2" t="str">
-        <f t="shared" ref="DW2" si="16">"0x"&amp;BIN2HEX(DW1,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="DX2" t="str">
-        <f t="shared" ref="DX2:ER2" si="17">"0x"&amp;BIN2HEX(DX1,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="DY2" t="str">
-        <f t="shared" si="17"/>
-        <v>0x00</v>
-      </c>
-      <c r="DZ2" t="str">
         <f t="shared" si="17"/>
         <v>0xFF</v>
       </c>
+      <c r="DU2" t="str">
+        <f t="shared" si="17"/>
+        <v>0x01</v>
+      </c>
+      <c r="DV2" t="str">
+        <f t="shared" si="17"/>
+        <v>0x01</v>
+      </c>
+      <c r="DW2" t="str">
+        <f t="shared" ref="DW2" si="18">"0x"&amp;BIN2HEX(DW1,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="DX2" t="str">
+        <f t="shared" ref="DX2:EM2" si="19">"0x"&amp;BIN2HEX(DX1,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="DY2" t="str">
+        <f t="shared" si="19"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DZ2" t="str">
+        <f t="shared" si="19"/>
+        <v>0x81</v>
+      </c>
       <c r="EA2" t="str">
-        <f t="shared" si="17"/>
-        <v>0x81</v>
+        <f t="shared" si="19"/>
+        <v>0x42</v>
       </c>
       <c r="EB2" t="str">
-        <f t="shared" si="17"/>
-        <v>0x42</v>
+        <f t="shared" si="19"/>
+        <v>0x3C</v>
       </c>
       <c r="EC2" t="str">
-        <f t="shared" si="17"/>
-        <v>0x3C</v>
+        <f t="shared" si="19"/>
+        <v>0x00</v>
       </c>
       <c r="ED2" t="str">
-        <f t="shared" si="17"/>
-        <v>0x00</v>
+        <f t="shared" si="19"/>
+        <v>0xF9</v>
       </c>
       <c r="EE2" t="str">
-        <f t="shared" si="17"/>
-        <v>0xF9</v>
+        <f t="shared" si="19"/>
+        <v>0x00</v>
       </c>
       <c r="EF2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EG2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EH2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EI2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EJ2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EK2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EL2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
       <c r="EM2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0x00</v>
       </c>
     </row>
@@ -2566,28 +2588,28 @@
       <c r="AM3" t="s">
         <v>0</v>
       </c>
-      <c r="AP3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ3" t="s">
+      <c r="AO3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2628,10 +2650,13 @@
       <c r="AM4" t="s">
         <v>0</v>
       </c>
-      <c r="AP4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS4" t="s">
+      <c r="AO4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="s">
         <v>0</v>
       </c>
       <c r="AU4" t="s">
@@ -2640,19 +2665,16 @@
       <c r="AV4" t="s">
         <v>0</v>
       </c>
-      <c r="AW4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ4" t="s">
+      <c r="AY4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2705,28 +2727,28 @@
       <c r="AM5" t="s">
         <v>0</v>
       </c>
-      <c r="AP5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS5" t="s">
+      <c r="AO5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="s">
         <v>0</v>
       </c>
       <c r="AU5" t="s">
         <v>0</v>
       </c>
-      <c r="AV5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ5" t="s">
+      <c r="AY5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2761,25 +2783,25 @@
       <c r="AM6" t="s">
         <v>0</v>
       </c>
-      <c r="AP6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH6" t="s">
+      <c r="AO6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2814,25 +2836,25 @@
       <c r="AM7" t="s">
         <v>0</v>
       </c>
-      <c r="AP7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>0</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG7" t="s">
+      <c r="AO7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF7" t="s">
         <v>0</v>
       </c>
       <c r="BW7" t="s">
@@ -2894,16 +2916,19 @@
       <c r="AL8" t="s">
         <v>0</v>
       </c>
+      <c r="AP8" t="s">
+        <v>0</v>
+      </c>
       <c r="AQ8" t="s">
         <v>0</v>
       </c>
-      <c r="AR8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX8" t="s">
+      <c r="AT8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="s">
         <v>0</v>
       </c>
       <c r="AZ8" t="s">
@@ -2915,16 +2940,13 @@
       <c r="BB8" t="s">
         <v>0</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BD8" t="s">
         <v>0</v>
       </c>
       <c r="BE8" t="s">
         <v>0</v>
       </c>
-      <c r="BF8" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ8" t="s">
+      <c r="BI8" t="s">
         <v>0</v>
       </c>
       <c r="BV8" t="s">
@@ -3159,7 +3181,7 @@
         <v>2</v>
       </c>
       <c r="BW10" t="str">
-        <f t="shared" ref="BW10:BW73" si="18">BW9&amp;" "&amp;BV10&amp;","</f>
+        <f t="shared" ref="BW10:BW73" si="20">BW9&amp;" "&amp;BV10&amp;","</f>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18,</v>
       </c>
     </row>
@@ -3378,7 +3400,7 @@
         <v>2</v>
       </c>
       <c r="BW11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18,</v>
       </c>
     </row>
@@ -3387,7 +3409,7 @@
         <v>9</v>
       </c>
       <c r="BW12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF,</v>
       </c>
     </row>
@@ -3396,7 +3418,7 @@
         <v>6</v>
       </c>
       <c r="BW13" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00,</v>
       </c>
     </row>
@@ -3405,7 +3427,7 @@
         <v>9</v>
       </c>
       <c r="BW14" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF,</v>
       </c>
     </row>
@@ -3414,7 +3436,7 @@
         <v>10</v>
       </c>
       <c r="BW15" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89,</v>
       </c>
     </row>
@@ -3423,7 +3445,7 @@
         <v>10</v>
       </c>
       <c r="BW16" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89,</v>
       </c>
     </row>
@@ -3432,7 +3454,7 @@
         <v>10</v>
       </c>
       <c r="BW17" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89,</v>
       </c>
     </row>
@@ -3441,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="BW18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00,</v>
       </c>
     </row>
@@ -3450,7 +3472,7 @@
         <v>9</v>
       </c>
       <c r="BW19" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF,</v>
       </c>
     </row>
@@ -3459,7 +3481,7 @@
         <v>11</v>
       </c>
       <c r="BW20" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01,</v>
       </c>
     </row>
@@ -3468,7 +3490,7 @@
         <v>11</v>
       </c>
       <c r="BW21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01,</v>
       </c>
     </row>
@@ -3477,7 +3499,7 @@
         <v>11</v>
       </c>
       <c r="BW22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
       </c>
     </row>
@@ -3486,7 +3508,7 @@
         <v>6</v>
       </c>
       <c r="BW23" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
       </c>
     </row>
@@ -3495,7 +3517,7 @@
         <v>9</v>
       </c>
       <c r="BW24" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
       </c>
     </row>
@@ -3504,7 +3526,7 @@
         <v>11</v>
       </c>
       <c r="BW25" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01,</v>
       </c>
     </row>
@@ -3513,7 +3535,7 @@
         <v>11</v>
       </c>
       <c r="BW26" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01,</v>
       </c>
     </row>
@@ -3522,7 +3544,7 @@
         <v>11</v>
       </c>
       <c r="BW27" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
       </c>
     </row>
@@ -3531,7 +3553,7 @@
         <v>6</v>
       </c>
       <c r="BW28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
       </c>
     </row>
@@ -3540,7 +3562,7 @@
         <v>12</v>
       </c>
       <c r="BW29" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E,</v>
       </c>
     </row>
@@ -3549,7 +3571,7 @@
         <v>5</v>
       </c>
       <c r="BW30" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81,</v>
       </c>
     </row>
@@ -3558,7 +3580,7 @@
         <v>5</v>
       </c>
       <c r="BW31" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81,</v>
       </c>
     </row>
@@ -3567,7 +3589,7 @@
         <v>12</v>
       </c>
       <c r="BW32" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
       </c>
     </row>
@@ -3576,7 +3598,7 @@
         <v>6</v>
       </c>
       <c r="BW33" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
       </c>
     </row>
@@ -3585,7 +3607,7 @@
         <v>6</v>
       </c>
       <c r="BW34" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3594,7 +3616,7 @@
         <v>6</v>
       </c>
       <c r="BW35" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3603,7 +3625,7 @@
         <v>6</v>
       </c>
       <c r="BW36" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3612,7 +3634,7 @@
         <v>6</v>
       </c>
       <c r="BW37" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3621,7 +3643,7 @@
         <v>6</v>
       </c>
       <c r="BW38" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3630,7 +3652,7 @@
         <v>6</v>
       </c>
       <c r="BW39" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3639,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="BW40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3648,7 +3670,7 @@
         <v>6</v>
       </c>
       <c r="BW41" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
@@ -3657,7 +3679,7 @@
         <v>19</v>
       </c>
       <c r="BW42" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE,</v>
       </c>
     </row>
@@ -3666,7 +3688,7 @@
         <v>11</v>
       </c>
       <c r="BW43" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01,</v>
       </c>
     </row>
@@ -3675,7 +3697,7 @@
         <v>20</v>
       </c>
       <c r="BW44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E,</v>
       </c>
     </row>
@@ -3684,7 +3706,7 @@
         <v>11</v>
       </c>
       <c r="BW45" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01,</v>
       </c>
     </row>
@@ -3693,7 +3715,7 @@
         <v>19</v>
       </c>
       <c r="BW46" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE,</v>
       </c>
     </row>
@@ -3702,26 +3724,26 @@
         <v>6</v>
       </c>
       <c r="BW47" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00,</v>
       </c>
     </row>
     <row r="48" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV48" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="BW48" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E,</v>
       </c>
     </row>
     <row r="49" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV49" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="BW49" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81,</v>
       </c>
     </row>
     <row r="50" spans="74:75" x14ac:dyDescent="0.25">
@@ -3729,89 +3751,89 @@
         <v>5</v>
       </c>
       <c r="BW50" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81,</v>
       </c>
     </row>
     <row r="51" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV51" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BW51" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
       </c>
     </row>
     <row r="52" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV52" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="BW52" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
       </c>
     </row>
     <row r="53" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV53" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BW53" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF,</v>
       </c>
     </row>
     <row r="54" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV54" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BW54" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98,</v>
       </c>
     </row>
     <row r="55" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BW55" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94,</v>
       </c>
     </row>
     <row r="56" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BW56" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63,</v>
       </c>
     </row>
     <row r="57" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV57" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BW57" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00,</v>
       </c>
     </row>
     <row r="58" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV58" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BW58" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF,</v>
       </c>
     </row>
     <row r="59" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV59" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BW59" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01,</v>
       </c>
     </row>
     <row r="60" spans="74:75" x14ac:dyDescent="0.25">
@@ -3819,8 +3841,8 @@
         <v>11</v>
       </c>
       <c r="BW60" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01,</v>
       </c>
     </row>
     <row r="61" spans="74:75" x14ac:dyDescent="0.25">
@@ -3828,80 +3850,80 @@
         <v>11</v>
       </c>
       <c r="BW61" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
       </c>
     </row>
     <row r="62" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV62" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BW62" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
       </c>
     </row>
     <row r="63" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BW63" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
       </c>
     </row>
     <row r="64" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV64" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="BW64" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81,</v>
       </c>
     </row>
     <row r="65" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BW65" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42,</v>
       </c>
     </row>
     <row r="66" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV66" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="BW66" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C,</v>
       </c>
     </row>
     <row r="67" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV67" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="BW67" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00,</v>
       </c>
     </row>
     <row r="68" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV68" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="BW68" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9,</v>
       </c>
     </row>
     <row r="69" spans="74:75" x14ac:dyDescent="0.25">
       <c r="BV69" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="BW69" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00,</v>
       </c>
     </row>
     <row r="70" spans="74:75" x14ac:dyDescent="0.25">
@@ -3909,8 +3931,8 @@
         <v>6</v>
       </c>
       <c r="BW70" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="71" spans="74:75" x14ac:dyDescent="0.25">
@@ -3918,8 +3940,8 @@
         <v>6</v>
       </c>
       <c r="BW71" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="72" spans="74:75" x14ac:dyDescent="0.25">
@@ -3927,8 +3949,8 @@
         <v>6</v>
       </c>
       <c r="BW72" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="73" spans="74:75" x14ac:dyDescent="0.25">
@@ -3936,8 +3958,8 @@
         <v>6</v>
       </c>
       <c r="BW73" t="str">
-        <f t="shared" si="18"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00,</v>
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="74" spans="74:75" x14ac:dyDescent="0.25">
@@ -3945,8 +3967,8 @@
         <v>6</v>
       </c>
       <c r="BW74" t="str">
-        <f t="shared" ref="BW74:BW77" si="19">BW73&amp;" "&amp;BV74&amp;","</f>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+        <f t="shared" ref="BW74:BW77" si="21">BW73&amp;" "&amp;BV74&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="75" spans="74:75" x14ac:dyDescent="0.25">
@@ -3954,8 +3976,8 @@
         <v>6</v>
       </c>
       <c r="BW75" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="76" spans="74:75" x14ac:dyDescent="0.25">
@@ -3963,8 +3985,8 @@
         <v>6</v>
       </c>
       <c r="BW76" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
     <row r="77" spans="74:75" x14ac:dyDescent="0.25">
@@ -3972,12 +3994,2332 @@
         <v>6</v>
       </c>
       <c r="BW77" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0x7E, 0x81, 0x81, 0x7E, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477C8103-FE84-45C6-A961-B22B68C061E8}">
+  <dimension ref="A1:EQ81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BX8" sqref="BX8:BX79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="2.140625" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="72" width="2.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX1" t="str">
+        <f>LEN(A1)&amp;LEN(A2)&amp;LEN(A3)&amp;LEN(A4)&amp;LEN(A5)&amp;LEN(A6)&amp;LEN(A7)&amp;LEN(A8)</f>
+        <v>11111110</v>
+      </c>
+      <c r="BY1" t="str">
+        <f t="shared" ref="BY1:EJ1" si="0">LEN(B1)&amp;LEN(B2)&amp;LEN(B3)&amp;LEN(B4)&amp;LEN(B5)&amp;LEN(B6)&amp;LEN(B7)&amp;LEN(B8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="BZ1" t="str">
+        <f t="shared" si="0"/>
+        <v>00001110</v>
+      </c>
+      <c r="CA1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="CB1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111110</v>
+      </c>
+      <c r="CC1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CD1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="CE1" t="str">
+        <f t="shared" si="0"/>
+        <v>00011000</v>
+      </c>
+      <c r="CF1" t="str">
+        <f t="shared" si="0"/>
+        <v>00011000</v>
+      </c>
+      <c r="CG1" t="str">
+        <f t="shared" si="0"/>
+        <v>00011000</v>
+      </c>
+      <c r="CH1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="CI1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CJ1" t="str">
+        <f t="shared" si="0"/>
+        <v>10000001</v>
+      </c>
+      <c r="CK1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="CL1" t="str">
+        <f t="shared" si="0"/>
+        <v>10000001</v>
+      </c>
+      <c r="CM1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CN1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="CO1" t="str">
+        <f t="shared" si="0"/>
+        <v>10011000</v>
+      </c>
+      <c r="CP1" t="str">
+        <f t="shared" si="0"/>
+        <v>10010100</v>
+      </c>
+      <c r="CQ1" t="str">
+        <f t="shared" si="0"/>
+        <v>01100011</v>
+      </c>
+      <c r="CR1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CS1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="CT1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CU1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="CV1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="CW1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="CX1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="CY1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="CZ1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="DA1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DB1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DC1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DD1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DE1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="DF1" t="str">
+        <f t="shared" si="0"/>
+        <v>10000001</v>
+      </c>
+      <c r="DG1" t="str">
+        <f t="shared" si="0"/>
+        <v>01000010</v>
+      </c>
+      <c r="DH1" t="str">
+        <f t="shared" si="0"/>
+        <v>00111100</v>
+      </c>
+      <c r="DI1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DJ1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DK1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DL1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DM1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DN1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="DO1" t="str">
+        <f t="shared" si="0"/>
+        <v>10010000</v>
+      </c>
+      <c r="DP1" t="str">
+        <f t="shared" si="0"/>
+        <v>10010000</v>
+      </c>
+      <c r="DQ1" t="str">
+        <f t="shared" si="0"/>
+        <v>01100000</v>
+      </c>
+      <c r="DR1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DS1" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="DT1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DU1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DV1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="DW1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DX1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="DY1" t="str">
+        <f t="shared" si="0"/>
+        <v>00011111</v>
+      </c>
+      <c r="DZ1" t="str">
+        <f t="shared" si="0"/>
+        <v>01101000</v>
+      </c>
+      <c r="EA1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001000</v>
+      </c>
+      <c r="EB1" t="str">
+        <f t="shared" si="0"/>
+        <v>01101000</v>
+      </c>
+      <c r="EC1" t="str">
+        <f t="shared" si="0"/>
+        <v>00011111</v>
+      </c>
+      <c r="ED1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="EE1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="EF1" t="str">
+        <f t="shared" si="0"/>
+        <v>01110010</v>
+      </c>
+      <c r="EG1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="EH1" t="str">
+        <f t="shared" si="0"/>
+        <v>10001001</v>
+      </c>
+      <c r="EI1" t="str">
+        <f t="shared" si="0"/>
+        <v>01000110</v>
+      </c>
+      <c r="EJ1" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="EK1" t="str">
+        <f t="shared" ref="EK1:EW1" si="1">LEN(BN1)&amp;LEN(BN2)&amp;LEN(BN3)&amp;LEN(BN4)&amp;LEN(BN5)&amp;LEN(BN6)&amp;LEN(BN7)&amp;LEN(BN8)</f>
+        <v>11111001</v>
+      </c>
+      <c r="EL1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="EM1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="EN1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="EO1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="EP1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="EQ1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX2" t="str">
+        <f t="shared" ref="BX2:EI2" si="2">"0x"&amp;BIN2HEX(BX1,2)</f>
+        <v>0xFE</v>
+      </c>
+      <c r="BY2" t="str">
+        <f t="shared" ref="BY2:EJ2" si="3">"0x"&amp;BIN2HEX(BY1,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="BZ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0E</v>
+      </c>
+      <c r="CA2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x01</v>
+      </c>
+      <c r="CB2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFE</v>
+      </c>
+      <c r="CC2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CD2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="CE2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x18</v>
+      </c>
+      <c r="CF2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x18</v>
+      </c>
+      <c r="CG2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x18</v>
+      </c>
+      <c r="CH2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="CI2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CJ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x81</v>
+      </c>
+      <c r="CK2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="CL2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x81</v>
+      </c>
+      <c r="CM2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CN2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="CO2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x98</v>
+      </c>
+      <c r="CP2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x94</v>
+      </c>
+      <c r="CQ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x63</v>
+      </c>
+      <c r="CR2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CS2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x01</v>
+      </c>
+      <c r="CT2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CU2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="CV2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x01</v>
+      </c>
+      <c r="CW2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x01</v>
+      </c>
+      <c r="CX2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x01</v>
+      </c>
+      <c r="CY2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="CZ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DA2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DB2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DC2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DD2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DE2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DF2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x81</v>
+      </c>
+      <c r="DG2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x42</v>
+      </c>
+      <c r="DH2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x3C</v>
+      </c>
+      <c r="DI2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DJ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DK2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DL2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DM2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DN2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DO2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x90</v>
+      </c>
+      <c r="DP2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x90</v>
+      </c>
+      <c r="DQ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x60</v>
+      </c>
+      <c r="DR2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DS2" t="str">
+        <f t="shared" si="3"/>
+        <v>0xFF</v>
+      </c>
+      <c r="DT2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DU2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DV2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="DW2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DX2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="DY2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x1F</v>
+      </c>
+      <c r="DZ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x68</v>
+      </c>
+      <c r="EA2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x88</v>
+      </c>
+      <c r="EB2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x68</v>
+      </c>
+      <c r="EC2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x1F</v>
+      </c>
+      <c r="ED2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="EE2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="EF2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x72</v>
+      </c>
+      <c r="EG2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="EH2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x89</v>
+      </c>
+      <c r="EI2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x46</v>
+      </c>
+      <c r="EJ2" t="str">
+        <f t="shared" si="3"/>
+        <v>0x00</v>
+      </c>
+      <c r="EK2" t="str">
+        <f t="shared" ref="EK2:EW2" si="4">"0x"&amp;BIN2HEX(EK1,2)</f>
+        <v>0xF9</v>
+      </c>
+      <c r="EL2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+      <c r="EM2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+      <c r="EN2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+      <c r="EO2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+      <c r="EP2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+      <c r="EQ2" t="str">
+        <f t="shared" si="4"/>
+        <v>0x00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>19</v>
+      </c>
+      <c r="BY8" t="str">
+        <f>BY7&amp;BX8&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY9" t="str">
+        <f>BY8&amp;" "&amp;BX9&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BX10" t="s">
+        <v>20</v>
+      </c>
+      <c r="BY10" t="str">
+        <f t="shared" ref="BY10:BY73" si="5">BY9&amp;" "&amp;BX10&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:147" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2">
+        <v>9</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10</v>
+      </c>
+      <c r="K11" s="2">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2">
+        <v>12</v>
+      </c>
+      <c r="M11" s="2">
+        <v>13</v>
+      </c>
+      <c r="N11" s="2">
+        <v>14</v>
+      </c>
+      <c r="O11" s="2">
+        <v>15</v>
+      </c>
+      <c r="P11" s="2">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>17</v>
+      </c>
+      <c r="R11" s="2">
+        <v>18</v>
+      </c>
+      <c r="S11" s="2">
+        <v>19</v>
+      </c>
+      <c r="T11" s="2">
+        <v>20</v>
+      </c>
+      <c r="U11" s="2">
+        <v>21</v>
+      </c>
+      <c r="V11" s="2">
+        <v>22</v>
+      </c>
+      <c r="W11" s="2">
+        <v>23</v>
+      </c>
+      <c r="X11" s="2">
+        <v>24</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>25</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>26</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>27</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>28</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>29</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>30</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>31</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>32</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>33</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>34</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>35</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>36</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>38</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>39</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>40</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>41</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>42</v>
+      </c>
+      <c r="AQ11" s="2">
+        <v>43</v>
+      </c>
+      <c r="AR11" s="2">
+        <v>44</v>
+      </c>
+      <c r="AS11" s="2">
+        <v>45</v>
+      </c>
+      <c r="AT11" s="2">
+        <v>46</v>
+      </c>
+      <c r="AU11" s="2">
+        <v>47</v>
+      </c>
+      <c r="AV11" s="2">
+        <v>48</v>
+      </c>
+      <c r="AW11" s="2">
+        <v>49</v>
+      </c>
+      <c r="AX11" s="2">
+        <v>50</v>
+      </c>
+      <c r="AY11" s="2">
+        <v>51</v>
+      </c>
+      <c r="AZ11" s="2">
+        <v>52</v>
+      </c>
+      <c r="BA11" s="2">
+        <v>53</v>
+      </c>
+      <c r="BB11" s="2">
+        <v>54</v>
+      </c>
+      <c r="BC11" s="2">
+        <v>55</v>
+      </c>
+      <c r="BD11" s="2">
+        <v>56</v>
+      </c>
+      <c r="BE11" s="2">
+        <v>57</v>
+      </c>
+      <c r="BF11" s="2">
+        <v>58</v>
+      </c>
+      <c r="BG11" s="2">
+        <v>59</v>
+      </c>
+      <c r="BH11" s="2">
+        <v>60</v>
+      </c>
+      <c r="BI11" s="2">
+        <v>61</v>
+      </c>
+      <c r="BJ11" s="2">
+        <v>62</v>
+      </c>
+      <c r="BK11" s="2">
+        <v>63</v>
+      </c>
+      <c r="BL11" s="2">
+        <v>64</v>
+      </c>
+      <c r="BM11" s="2">
+        <v>65</v>
+      </c>
+      <c r="BN11" s="2">
+        <v>66</v>
+      </c>
+      <c r="BO11" s="2">
+        <v>67</v>
+      </c>
+      <c r="BP11" s="2">
+        <v>68</v>
+      </c>
+      <c r="BQ11" s="2">
+        <v>69</v>
+      </c>
+      <c r="BR11" s="2">
+        <v>70</v>
+      </c>
+      <c r="BS11" s="2">
+        <v>71</v>
+      </c>
+      <c r="BT11" s="2">
+        <v>72</v>
+      </c>
+      <c r="BV11" s="2"/>
+      <c r="BX11" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BV12" s="2"/>
+      <c r="BX12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BY12" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BV13" s="2"/>
+      <c r="BX13" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY13" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BV14" s="2"/>
+      <c r="BX14" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY14" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BV15" s="2"/>
+      <c r="BX15" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY15" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="BV16" s="2"/>
+      <c r="BX16" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY16" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18,</v>
+      </c>
+    </row>
+    <row r="17" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV17" s="2"/>
+      <c r="BX17" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY17" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18,</v>
+      </c>
+    </row>
+    <row r="18" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV18" s="2"/>
+      <c r="BX18" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY18" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF,</v>
+      </c>
+    </row>
+    <row r="19" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV19" s="2"/>
+      <c r="BX19" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY19" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00,</v>
+      </c>
+    </row>
+    <row r="20" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV20" s="2"/>
+      <c r="BX20" t="s">
+        <v>5</v>
+      </c>
+      <c r="BY20" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81,</v>
+      </c>
+    </row>
+    <row r="21" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV21" s="2"/>
+      <c r="BX21" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY21" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF,</v>
+      </c>
+    </row>
+    <row r="22" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV22" s="2"/>
+      <c r="BX22" t="s">
+        <v>5</v>
+      </c>
+      <c r="BY22" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81,</v>
+      </c>
+    </row>
+    <row r="23" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV23" s="2"/>
+      <c r="BX23" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY23" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00,</v>
+      </c>
+    </row>
+    <row r="24" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV24" s="2"/>
+      <c r="BX24" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY24" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="25" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV25" s="2"/>
+      <c r="BX25" t="s">
+        <v>13</v>
+      </c>
+      <c r="BY25" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98,</v>
+      </c>
+    </row>
+    <row r="26" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV26" s="2"/>
+      <c r="BX26" t="s">
+        <v>14</v>
+      </c>
+      <c r="BY26" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94,</v>
+      </c>
+    </row>
+    <row r="27" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV27" s="2"/>
+      <c r="BX27" t="s">
+        <v>15</v>
+      </c>
+      <c r="BY27" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63,</v>
+      </c>
+    </row>
+    <row r="28" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV28" s="2"/>
+      <c r="BX28" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY28" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00,</v>
+      </c>
+    </row>
+    <row r="29" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV29" s="2"/>
+      <c r="BX29" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY29" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01,</v>
+      </c>
+    </row>
+    <row r="30" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV30" s="2"/>
+      <c r="BX30" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY30" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00,</v>
+      </c>
+    </row>
+    <row r="31" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV31" s="2"/>
+      <c r="BX31" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY31" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="32" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV32" s="2"/>
+      <c r="BX32" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY32" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01,</v>
+      </c>
+    </row>
+    <row r="33" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV33" s="2"/>
+      <c r="BX33" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY33" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="34" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV34" s="2"/>
+      <c r="BX34" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY34" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01,</v>
+      </c>
+    </row>
+    <row r="35" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV35" s="2"/>
+      <c r="BX35" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY35" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00,</v>
+      </c>
+    </row>
+    <row r="36" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV36" s="2"/>
+      <c r="BX36" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY36" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="37" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV37" s="2"/>
+      <c r="BX37" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY37" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89,</v>
+      </c>
+    </row>
+    <row r="38" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV38" s="2"/>
+      <c r="BX38" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY38" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="39" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV39" s="2"/>
+      <c r="BX39" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY39" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="40" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV40" s="2"/>
+      <c r="BX40" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00,</v>
+      </c>
+    </row>
+    <row r="41" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV41" s="2"/>
+      <c r="BX41" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY41" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="42" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV42" s="2"/>
+      <c r="BX42" t="s">
+        <v>5</v>
+      </c>
+      <c r="BY42" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81,</v>
+      </c>
+    </row>
+    <row r="43" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV43" s="2"/>
+      <c r="BX43" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY43" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42,</v>
+      </c>
+    </row>
+    <row r="44" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV44" s="2"/>
+      <c r="BX44" t="s">
+        <v>16</v>
+      </c>
+      <c r="BY44" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C,</v>
+      </c>
+    </row>
+    <row r="45" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV45" s="2"/>
+      <c r="BX45" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY45" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00,</v>
+      </c>
+    </row>
+    <row r="46" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV46" s="2"/>
+      <c r="BX46" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY46" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="47" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV47" s="2"/>
+      <c r="BX47" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY47" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="48" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV48" s="2"/>
+      <c r="BX48" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY48" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="49" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV49" s="2"/>
+      <c r="BX49" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY49" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="50" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV50" s="2"/>
+      <c r="BX50" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY50" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="51" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV51" s="2"/>
+      <c r="BX51" t="s">
+        <v>24</v>
+      </c>
+      <c r="BY51" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90,</v>
+      </c>
+    </row>
+    <row r="52" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV52" s="2"/>
+      <c r="BX52" t="s">
+        <v>24</v>
+      </c>
+      <c r="BY52" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90,</v>
+      </c>
+    </row>
+    <row r="53" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV53" s="2"/>
+      <c r="BX53" t="s">
+        <v>25</v>
+      </c>
+      <c r="BY53" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60,</v>
+      </c>
+    </row>
+    <row r="54" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV54" s="2"/>
+      <c r="BX54" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY54" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00,</v>
+      </c>
+    </row>
+    <row r="55" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV55" s="2"/>
+      <c r="BX55" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY55" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF,</v>
+      </c>
+    </row>
+    <row r="56" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV56" s="2"/>
+      <c r="BX56" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY56" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89,</v>
+      </c>
+    </row>
+    <row r="57" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV57" s="2"/>
+      <c r="BX57" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY57" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="58" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV58" s="2"/>
+      <c r="BX58" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY58" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="59" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV59" s="2"/>
+      <c r="BX59" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY59" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00,</v>
+      </c>
+    </row>
+    <row r="60" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV60" s="2"/>
+      <c r="BX60" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY60" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="61" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV61" s="2"/>
+      <c r="BX61" t="s">
+        <v>26</v>
+      </c>
+      <c r="BY61" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F,</v>
+      </c>
+    </row>
+    <row r="62" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV62" s="2"/>
+      <c r="BX62" t="s">
+        <v>27</v>
+      </c>
+      <c r="BY62" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68,</v>
+      </c>
+    </row>
+    <row r="63" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV63" s="2"/>
+      <c r="BX63" t="s">
+        <v>28</v>
+      </c>
+      <c r="BY63" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88,</v>
+      </c>
+    </row>
+    <row r="64" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV64" s="2"/>
+      <c r="BX64" t="s">
+        <v>27</v>
+      </c>
+      <c r="BY64" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68,</v>
+      </c>
+    </row>
+    <row r="65" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV65" s="2"/>
+      <c r="BX65" t="s">
+        <v>26</v>
+      </c>
+      <c r="BY65" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F,</v>
+      </c>
+    </row>
+    <row r="66" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV66" s="2"/>
+      <c r="BX66" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY66" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00,</v>
+      </c>
+    </row>
+    <row r="67" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV67" s="2"/>
+      <c r="BX67" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY67" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="68" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV68" s="2"/>
+      <c r="BX68" t="s">
+        <v>29</v>
+      </c>
+      <c r="BY68" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72,</v>
+      </c>
+    </row>
+    <row r="69" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV69" s="2"/>
+      <c r="BX69" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY69" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89,</v>
+      </c>
+    </row>
+    <row r="70" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV70" s="2"/>
+      <c r="BX70" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY70" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89,</v>
+      </c>
+    </row>
+    <row r="71" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV71" s="2"/>
+      <c r="BX71" t="s">
+        <v>30</v>
+      </c>
+      <c r="BY71" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46,</v>
+      </c>
+    </row>
+    <row r="72" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV72" s="2"/>
+      <c r="BX72" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY72" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00,</v>
+      </c>
+    </row>
+    <row r="73" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV73" s="2"/>
+      <c r="BX73" t="s">
+        <v>17</v>
+      </c>
+      <c r="BY73" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9,</v>
+      </c>
+    </row>
+    <row r="74" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV74" s="2"/>
+      <c r="BX74" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY74" t="str">
+        <f t="shared" ref="BY74:BY79" si="6">BY73&amp;" "&amp;BX74&amp;","</f>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00,</v>
+      </c>
+    </row>
+    <row r="75" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV75" s="2"/>
+      <c r="BX75" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY75" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="76" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV76" s="2"/>
+      <c r="BX76" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY76" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="77" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV77" s="2"/>
+      <c r="BX77" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY77" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="78" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV78" s="2"/>
+      <c r="BX78" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY78" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="79" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV79" s="2"/>
+      <c r="BX79" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY79" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  static unsigned int hello_pattern[PTRN_CALLS_THEN_REPEAT] = { 0xFE, 0x01, 0x0E, 0x01, 0xFE, 0x00, 0xFF, 0x18, 0x18, 0x18, 0xFF, 0x00, 0x81, 0xFF, 0x81, 0x00, 0xFF, 0x98, 0x94, 0x63, 0x00, 0x01, 0x00, 0xFF, 0x01, 0x01, 0x01, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0xFF, 0x81, 0x42, 0x3C, 0x00, 0x00, 0x00, 0x00, 0x00, 0xFF, 0x90, 0x90, 0x60, 0x00, 0xFF, 0x89, 0x89, 0x89, 0x00, 0x00, 0x1F, 0x68, 0x88, 0x68, 0x1F, 0x00, 0x00, 0x72, 0x89, 0x89, 0x46, 0x00, 0xF9, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
+      </c>
+    </row>
+    <row r="80" spans="74:77" x14ac:dyDescent="0.25">
+      <c r="BV80" s="2"/>
+    </row>
+    <row r="81" spans="74:74" x14ac:dyDescent="0.25">
+      <c r="BV81" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>